<commit_message>
Fixed outfting formula on template
</commit_message>
<xml_diff>
--- a/CostingSheetTemplate.xlsx
+++ b/CostingSheetTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developer\samples\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\nrb-costing-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -916,7 +916,14 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1289,9 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J461"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3447,14 +3452,14 @@
         <v>9</v>
       </c>
       <c r="G108" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="G108:G171" si="14">F108*D108</f>
         <v>0</v>
       </c>
       <c r="H108" s="9">
         <v>0</v>
       </c>
       <c r="I108" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="I108:I171" si="15">H108+G108</f>
         <v>0</v>
       </c>
     </row>
@@ -3469,14 +3474,14 @@
         <v>9</v>
       </c>
       <c r="G109" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H109" s="9">
         <v>0</v>
       </c>
       <c r="I109" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3491,14 +3496,14 @@
         <v>9</v>
       </c>
       <c r="G110" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H110" s="9">
         <v>0</v>
       </c>
       <c r="I110" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3513,14 +3518,14 @@
         <v>9</v>
       </c>
       <c r="G111" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H111" s="9">
         <v>0</v>
       </c>
       <c r="I111" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3535,14 +3540,14 @@
         <v>9</v>
       </c>
       <c r="G112" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H112" s="9">
         <v>0</v>
       </c>
       <c r="I112" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3557,14 +3562,14 @@
         <v>9</v>
       </c>
       <c r="G113" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H113" s="9">
         <v>0</v>
       </c>
       <c r="I113" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3579,14 +3584,14 @@
         <v>9</v>
       </c>
       <c r="G114" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H114" s="9">
         <v>0</v>
       </c>
       <c r="I114" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3601,14 +3606,14 @@
         <v>9</v>
       </c>
       <c r="G115" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H115" s="9">
         <v>0</v>
       </c>
       <c r="I115" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3623,14 +3628,14 @@
         <v>9</v>
       </c>
       <c r="G116" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H116" s="9">
         <v>0</v>
       </c>
       <c r="I116" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3645,14 +3650,14 @@
         <v>9</v>
       </c>
       <c r="G117" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H117" s="9">
         <v>0</v>
       </c>
       <c r="I117" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3667,14 +3672,14 @@
         <v>9</v>
       </c>
       <c r="G118" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H118" s="9">
         <v>0</v>
       </c>
       <c r="I118" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3689,14 +3694,14 @@
         <v>9</v>
       </c>
       <c r="G119" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H119" s="9">
         <v>0</v>
       </c>
       <c r="I119" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3711,14 +3716,14 @@
         <v>9</v>
       </c>
       <c r="G120" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H120" s="9">
         <v>0</v>
       </c>
       <c r="I120" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3733,14 +3738,14 @@
         <v>9</v>
       </c>
       <c r="G121" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H121" s="9">
         <v>0</v>
       </c>
       <c r="I121" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3755,14 +3760,14 @@
         <v>9</v>
       </c>
       <c r="G122" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H122" s="9">
         <v>0</v>
       </c>
       <c r="I122" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3777,14 +3782,14 @@
         <v>9</v>
       </c>
       <c r="G123" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H123" s="9">
         <v>0</v>
       </c>
       <c r="I123" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3799,14 +3804,14 @@
         <v>9</v>
       </c>
       <c r="G124" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H124" s="9">
         <v>0</v>
       </c>
       <c r="I124" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3821,14 +3826,14 @@
         <v>9</v>
       </c>
       <c r="G125" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H125" s="9">
         <v>0</v>
       </c>
       <c r="I125" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3843,14 +3848,14 @@
         <v>9</v>
       </c>
       <c r="G126" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H126" s="9">
         <v>0</v>
       </c>
       <c r="I126" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3865,14 +3870,14 @@
         <v>9</v>
       </c>
       <c r="G127" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H127" s="9">
         <v>0</v>
       </c>
       <c r="I127" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3887,14 +3892,14 @@
         <v>9</v>
       </c>
       <c r="G128" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H128" s="9">
         <v>0</v>
       </c>
       <c r="I128" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3909,14 +3914,14 @@
         <v>9</v>
       </c>
       <c r="G129" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H129" s="9">
         <v>0</v>
       </c>
       <c r="I129" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3931,14 +3936,14 @@
         <v>9</v>
       </c>
       <c r="G130" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H130" s="9">
         <v>0</v>
       </c>
       <c r="I130" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3953,14 +3958,14 @@
         <v>9</v>
       </c>
       <c r="G131" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H131" s="9">
         <v>0</v>
       </c>
       <c r="I131" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3975,14 +3980,14 @@
         <v>9</v>
       </c>
       <c r="G132" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H132" s="9">
         <v>0</v>
       </c>
       <c r="I132" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -3997,14 +4002,14 @@
         <v>9</v>
       </c>
       <c r="G133" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H133" s="9">
         <v>0</v>
       </c>
       <c r="I133" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4019,14 +4024,14 @@
         <v>9</v>
       </c>
       <c r="G134" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H134" s="9">
         <v>0</v>
       </c>
       <c r="I134" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4041,14 +4046,14 @@
         <v>9</v>
       </c>
       <c r="G135" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H135" s="9">
         <v>0</v>
       </c>
       <c r="I135" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4063,14 +4068,14 @@
         <v>9</v>
       </c>
       <c r="G136" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H136" s="9">
         <v>0</v>
       </c>
       <c r="I136" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4085,14 +4090,14 @@
         <v>9</v>
       </c>
       <c r="G137" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H137" s="9">
         <v>0</v>
       </c>
       <c r="I137" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4107,14 +4112,14 @@
         <v>9</v>
       </c>
       <c r="G138" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H138" s="9">
         <v>0</v>
       </c>
       <c r="I138" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4129,14 +4134,14 @@
         <v>9</v>
       </c>
       <c r="G139" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H139" s="9">
         <v>0</v>
       </c>
       <c r="I139" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4151,14 +4156,14 @@
         <v>9</v>
       </c>
       <c r="G140" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H140" s="9">
         <v>0</v>
       </c>
       <c r="I140" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4173,14 +4178,14 @@
         <v>9</v>
       </c>
       <c r="G141" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H141" s="9">
         <v>0</v>
       </c>
       <c r="I141" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4195,14 +4200,14 @@
         <v>9</v>
       </c>
       <c r="G142" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H142" s="9">
         <v>0</v>
       </c>
       <c r="I142" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4217,14 +4222,14 @@
         <v>9</v>
       </c>
       <c r="G143" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H143" s="9">
         <v>0</v>
       </c>
       <c r="I143" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4239,14 +4244,14 @@
         <v>9</v>
       </c>
       <c r="G144" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H144" s="9">
         <v>0</v>
       </c>
       <c r="I144" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4261,14 +4266,14 @@
         <v>9</v>
       </c>
       <c r="G145" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H145" s="9">
         <v>0</v>
       </c>
       <c r="I145" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4283,14 +4288,14 @@
         <v>9</v>
       </c>
       <c r="G146" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H146" s="9">
         <v>0</v>
       </c>
       <c r="I146" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4305,14 +4310,14 @@
         <v>9</v>
       </c>
       <c r="G147" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H147" s="9">
         <v>0</v>
       </c>
       <c r="I147" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4327,14 +4332,14 @@
         <v>9</v>
       </c>
       <c r="G148" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H148" s="9">
         <v>0</v>
       </c>
       <c r="I148" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4349,14 +4354,14 @@
         <v>9</v>
       </c>
       <c r="G149" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H149" s="9">
         <v>0</v>
       </c>
       <c r="I149" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4371,14 +4376,14 @@
         <v>9</v>
       </c>
       <c r="G150" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H150" s="9">
         <v>0</v>
       </c>
       <c r="I150" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4393,14 +4398,14 @@
         <v>9</v>
       </c>
       <c r="G151" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H151" s="9">
         <v>0</v>
       </c>
       <c r="I151" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4415,14 +4420,14 @@
         <v>9</v>
       </c>
       <c r="G152" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H152" s="9">
         <v>0</v>
       </c>
       <c r="I152" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4437,14 +4442,14 @@
         <v>9</v>
       </c>
       <c r="G153" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H153" s="9">
         <v>0</v>
       </c>
       <c r="I153" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4459,14 +4464,14 @@
         <v>9</v>
       </c>
       <c r="G154" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H154" s="9">
         <v>0</v>
       </c>
       <c r="I154" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4481,14 +4486,14 @@
         <v>9</v>
       </c>
       <c r="G155" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H155" s="9">
         <v>0</v>
       </c>
       <c r="I155" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4503,14 +4508,14 @@
         <v>9</v>
       </c>
       <c r="G156" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H156" s="9">
         <v>0</v>
       </c>
       <c r="I156" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4525,14 +4530,14 @@
         <v>9</v>
       </c>
       <c r="G157" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H157" s="9">
         <v>0</v>
       </c>
       <c r="I157" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4547,14 +4552,14 @@
         <v>9</v>
       </c>
       <c r="G158" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H158" s="9">
         <v>0</v>
       </c>
       <c r="I158" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4569,14 +4574,14 @@
         <v>9</v>
       </c>
       <c r="G159" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H159" s="9">
         <v>0</v>
       </c>
       <c r="I159" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4591,14 +4596,14 @@
         <v>9</v>
       </c>
       <c r="G160" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H160" s="9">
         <v>0</v>
       </c>
       <c r="I160" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4613,14 +4618,14 @@
         <v>9</v>
       </c>
       <c r="G161" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H161" s="9">
         <v>0</v>
       </c>
       <c r="I161" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4635,14 +4640,14 @@
         <v>9</v>
       </c>
       <c r="G162" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H162" s="9">
         <v>0</v>
       </c>
       <c r="I162" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4657,14 +4662,14 @@
         <v>9</v>
       </c>
       <c r="G163" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H163" s="9">
         <v>0</v>
       </c>
       <c r="I163" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4679,14 +4684,14 @@
         <v>9</v>
       </c>
       <c r="G164" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H164" s="9">
         <v>0</v>
       </c>
       <c r="I164" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4701,14 +4706,14 @@
         <v>9</v>
       </c>
       <c r="G165" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H165" s="9">
         <v>0</v>
       </c>
       <c r="I165" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4723,14 +4728,14 @@
         <v>9</v>
       </c>
       <c r="G166" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H166" s="9">
         <v>0</v>
       </c>
       <c r="I166" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4745,14 +4750,14 @@
         <v>9</v>
       </c>
       <c r="G167" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H167" s="9">
         <v>0</v>
       </c>
       <c r="I167" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4767,14 +4772,14 @@
         <v>9</v>
       </c>
       <c r="G168" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H168" s="9">
         <v>0</v>
       </c>
       <c r="I168" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4789,14 +4794,14 @@
         <v>9</v>
       </c>
       <c r="G169" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H169" s="9">
         <v>0</v>
       </c>
       <c r="I169" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4811,14 +4816,14 @@
         <v>9</v>
       </c>
       <c r="G170" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H170" s="9">
         <v>0</v>
       </c>
       <c r="I170" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4833,14 +4838,14 @@
         <v>9</v>
       </c>
       <c r="G171" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="H171" s="9">
         <v>0</v>
       </c>
       <c r="I171" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
     </row>
@@ -4855,14 +4860,14 @@
         <v>9</v>
       </c>
       <c r="G172" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="G172:G235" si="16">F172*D172</f>
         <v>0</v>
       </c>
       <c r="H172" s="9">
         <v>0</v>
       </c>
       <c r="I172" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="I172:I235" si="17">H172+G172</f>
         <v>0</v>
       </c>
     </row>
@@ -4877,14 +4882,14 @@
         <v>9</v>
       </c>
       <c r="G173" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H173" s="9">
         <v>0</v>
       </c>
       <c r="I173" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4899,14 +4904,14 @@
         <v>9</v>
       </c>
       <c r="G174" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H174" s="9">
         <v>0</v>
       </c>
       <c r="I174" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4921,14 +4926,14 @@
         <v>9</v>
       </c>
       <c r="G175" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H175" s="9">
         <v>0</v>
       </c>
       <c r="I175" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4943,14 +4948,14 @@
         <v>9</v>
       </c>
       <c r="G176" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H176" s="9">
         <v>0</v>
       </c>
       <c r="I176" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4965,14 +4970,14 @@
         <v>9</v>
       </c>
       <c r="G177" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H177" s="9">
         <v>0</v>
       </c>
       <c r="I177" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -4987,14 +4992,14 @@
         <v>9</v>
       </c>
       <c r="G178" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H178" s="9">
         <v>0</v>
       </c>
       <c r="I178" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5009,14 +5014,14 @@
         <v>9</v>
       </c>
       <c r="G179" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H179" s="9">
         <v>0</v>
       </c>
       <c r="I179" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5031,14 +5036,14 @@
         <v>9</v>
       </c>
       <c r="G180" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H180" s="9">
         <v>0</v>
       </c>
       <c r="I180" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5053,14 +5058,14 @@
         <v>9</v>
       </c>
       <c r="G181" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H181" s="9">
         <v>0</v>
       </c>
       <c r="I181" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5075,14 +5080,14 @@
         <v>9</v>
       </c>
       <c r="G182" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H182" s="9">
         <v>0</v>
       </c>
       <c r="I182" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5097,14 +5102,14 @@
         <v>9</v>
       </c>
       <c r="G183" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H183" s="9">
         <v>0</v>
       </c>
       <c r="I183" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5119,14 +5124,14 @@
         <v>9</v>
       </c>
       <c r="G184" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H184" s="9">
         <v>0</v>
       </c>
       <c r="I184" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5141,14 +5146,14 @@
         <v>9</v>
       </c>
       <c r="G185" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H185" s="9">
         <v>0</v>
       </c>
       <c r="I185" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5163,14 +5168,14 @@
         <v>9</v>
       </c>
       <c r="G186" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H186" s="9">
         <v>0</v>
       </c>
       <c r="I186" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5185,14 +5190,14 @@
         <v>9</v>
       </c>
       <c r="G187" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H187" s="9">
         <v>0</v>
       </c>
       <c r="I187" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5207,14 +5212,14 @@
         <v>9</v>
       </c>
       <c r="G188" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H188" s="9">
         <v>0</v>
       </c>
       <c r="I188" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5229,14 +5234,14 @@
         <v>9</v>
       </c>
       <c r="G189" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H189" s="9">
         <v>0</v>
       </c>
       <c r="I189" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5251,14 +5256,14 @@
         <v>9</v>
       </c>
       <c r="G190" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H190" s="9">
         <v>0</v>
       </c>
       <c r="I190" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5273,14 +5278,14 @@
         <v>9</v>
       </c>
       <c r="G191" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H191" s="9">
         <v>0</v>
       </c>
       <c r="I191" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5295,14 +5300,14 @@
         <v>9</v>
       </c>
       <c r="G192" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H192" s="9">
         <v>0</v>
       </c>
       <c r="I192" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5317,14 +5322,14 @@
         <v>9</v>
       </c>
       <c r="G193" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H193" s="9">
         <v>0</v>
       </c>
       <c r="I193" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5339,14 +5344,14 @@
         <v>9</v>
       </c>
       <c r="G194" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H194" s="9">
         <v>0</v>
       </c>
       <c r="I194" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5361,14 +5366,14 @@
         <v>9</v>
       </c>
       <c r="G195" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H195" s="9">
         <v>0</v>
       </c>
       <c r="I195" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5383,14 +5388,14 @@
         <v>9</v>
       </c>
       <c r="G196" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H196" s="9">
         <v>0</v>
       </c>
       <c r="I196" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5405,14 +5410,14 @@
         <v>9</v>
       </c>
       <c r="G197" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H197" s="9">
         <v>0</v>
       </c>
       <c r="I197" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5427,14 +5432,14 @@
         <v>9</v>
       </c>
       <c r="G198" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H198" s="9">
         <v>0</v>
       </c>
       <c r="I198" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5449,14 +5454,14 @@
         <v>9</v>
       </c>
       <c r="G199" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H199" s="9">
         <v>0</v>
       </c>
       <c r="I199" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5471,14 +5476,14 @@
         <v>9</v>
       </c>
       <c r="G200" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H200" s="9">
         <v>0</v>
       </c>
       <c r="I200" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5493,14 +5498,14 @@
         <v>9</v>
       </c>
       <c r="G201" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H201" s="9">
         <v>0</v>
       </c>
       <c r="I201" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5515,14 +5520,14 @@
         <v>9</v>
       </c>
       <c r="G202" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H202" s="9">
         <v>0</v>
       </c>
       <c r="I202" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5537,14 +5542,14 @@
         <v>9</v>
       </c>
       <c r="G203" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H203" s="9">
         <v>0</v>
       </c>
       <c r="I203" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5559,14 +5564,14 @@
         <v>9</v>
       </c>
       <c r="G204" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H204" s="9">
         <v>0</v>
       </c>
       <c r="I204" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5581,14 +5586,14 @@
         <v>9</v>
       </c>
       <c r="G205" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H205" s="9">
         <v>0</v>
       </c>
       <c r="I205" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5603,14 +5608,14 @@
         <v>9</v>
       </c>
       <c r="G206" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H206" s="9">
         <v>0</v>
       </c>
       <c r="I206" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5625,14 +5630,14 @@
         <v>9</v>
       </c>
       <c r="G207" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H207" s="9">
         <v>0</v>
       </c>
       <c r="I207" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5647,14 +5652,14 @@
         <v>9</v>
       </c>
       <c r="G208" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H208" s="9">
         <v>0</v>
       </c>
       <c r="I208" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5669,14 +5674,14 @@
         <v>9</v>
       </c>
       <c r="G209" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H209" s="9">
         <v>0</v>
       </c>
       <c r="I209" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5691,14 +5696,14 @@
         <v>9</v>
       </c>
       <c r="G210" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H210" s="9">
         <v>0</v>
       </c>
       <c r="I210" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5713,14 +5718,14 @@
         <v>9</v>
       </c>
       <c r="G211" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H211" s="9">
         <v>0</v>
       </c>
       <c r="I211" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5735,14 +5740,14 @@
         <v>9</v>
       </c>
       <c r="G212" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H212" s="9">
         <v>0</v>
       </c>
       <c r="I212" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5757,14 +5762,14 @@
         <v>9</v>
       </c>
       <c r="G213" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H213" s="9">
         <v>0</v>
       </c>
       <c r="I213" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5779,14 +5784,14 @@
         <v>9</v>
       </c>
       <c r="G214" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H214" s="9">
         <v>0</v>
       </c>
       <c r="I214" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5801,14 +5806,14 @@
         <v>9</v>
       </c>
       <c r="G215" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H215" s="9">
         <v>0</v>
       </c>
       <c r="I215" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5823,14 +5828,14 @@
         <v>9</v>
       </c>
       <c r="G216" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H216" s="9">
         <v>0</v>
       </c>
       <c r="I216" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5845,14 +5850,14 @@
         <v>9</v>
       </c>
       <c r="G217" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H217" s="9">
         <v>0</v>
       </c>
       <c r="I217" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5867,14 +5872,14 @@
         <v>9</v>
       </c>
       <c r="G218" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H218" s="9">
         <v>0</v>
       </c>
       <c r="I218" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5889,14 +5894,14 @@
         <v>9</v>
       </c>
       <c r="G219" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H219" s="9">
         <v>0</v>
       </c>
       <c r="I219" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5911,14 +5916,14 @@
         <v>9</v>
       </c>
       <c r="G220" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H220" s="9">
         <v>0</v>
       </c>
       <c r="I220" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5933,14 +5938,14 @@
         <v>9</v>
       </c>
       <c r="G221" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H221" s="9">
         <v>0</v>
       </c>
       <c r="I221" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5955,14 +5960,14 @@
         <v>9</v>
       </c>
       <c r="G222" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H222" s="9">
         <v>0</v>
       </c>
       <c r="I222" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5977,14 +5982,14 @@
         <v>9</v>
       </c>
       <c r="G223" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H223" s="9">
         <v>0</v>
       </c>
       <c r="I223" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -5999,14 +6004,14 @@
         <v>9</v>
       </c>
       <c r="G224" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H224" s="9">
         <v>0</v>
       </c>
       <c r="I224" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6021,14 +6026,14 @@
         <v>9</v>
       </c>
       <c r="G225" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H225" s="9">
         <v>0</v>
       </c>
       <c r="I225" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6043,14 +6048,14 @@
         <v>9</v>
       </c>
       <c r="G226" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H226" s="9">
         <v>0</v>
       </c>
       <c r="I226" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6065,14 +6070,14 @@
         <v>9</v>
       </c>
       <c r="G227" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H227" s="9">
         <v>0</v>
       </c>
       <c r="I227" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6087,14 +6092,14 @@
         <v>9</v>
       </c>
       <c r="G228" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H228" s="9">
         <v>0</v>
       </c>
       <c r="I228" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6109,14 +6114,14 @@
         <v>9</v>
       </c>
       <c r="G229" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H229" s="9">
         <v>0</v>
       </c>
       <c r="I229" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6131,14 +6136,14 @@
         <v>9</v>
       </c>
       <c r="G230" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H230" s="9">
         <v>0</v>
       </c>
       <c r="I230" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6153,14 +6158,14 @@
         <v>9</v>
       </c>
       <c r="G231" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H231" s="9">
         <v>0</v>
       </c>
       <c r="I231" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6175,14 +6180,14 @@
         <v>9</v>
       </c>
       <c r="G232" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H232" s="9">
         <v>0</v>
       </c>
       <c r="I232" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6197,14 +6202,14 @@
         <v>9</v>
       </c>
       <c r="G233" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H233" s="9">
         <v>0</v>
       </c>
       <c r="I233" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6219,14 +6224,14 @@
         <v>9</v>
       </c>
       <c r="G234" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H234" s="9">
         <v>0</v>
       </c>
       <c r="I234" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6241,14 +6246,14 @@
         <v>9</v>
       </c>
       <c r="G235" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H235" s="9">
         <v>0</v>
       </c>
       <c r="I235" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
@@ -6263,14 +6268,14 @@
         <v>9</v>
       </c>
       <c r="G236" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="G236:G299" si="18">F236*D236</f>
         <v>0</v>
       </c>
       <c r="H236" s="9">
         <v>0</v>
       </c>
       <c r="I236" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="I236:I299" si="19">H236+G236</f>
         <v>0</v>
       </c>
     </row>
@@ -6285,14 +6290,14 @@
         <v>9</v>
       </c>
       <c r="G237" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H237" s="9">
         <v>0</v>
       </c>
       <c r="I237" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6307,14 +6312,14 @@
         <v>9</v>
       </c>
       <c r="G238" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H238" s="9">
         <v>0</v>
       </c>
       <c r="I238" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6329,14 +6334,14 @@
         <v>9</v>
       </c>
       <c r="G239" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H239" s="9">
         <v>0</v>
       </c>
       <c r="I239" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6351,14 +6356,14 @@
         <v>9</v>
       </c>
       <c r="G240" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H240" s="9">
         <v>0</v>
       </c>
       <c r="I240" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6373,14 +6378,14 @@
         <v>9</v>
       </c>
       <c r="G241" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H241" s="9">
         <v>0</v>
       </c>
       <c r="I241" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6395,14 +6400,14 @@
         <v>9</v>
       </c>
       <c r="G242" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H242" s="9">
         <v>0</v>
       </c>
       <c r="I242" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6417,14 +6422,14 @@
         <v>9</v>
       </c>
       <c r="G243" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H243" s="9">
         <v>0</v>
       </c>
       <c r="I243" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6439,14 +6444,14 @@
         <v>9</v>
       </c>
       <c r="G244" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H244" s="9">
         <v>0</v>
       </c>
       <c r="I244" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6461,14 +6466,14 @@
         <v>9</v>
       </c>
       <c r="G245" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H245" s="9">
         <v>0</v>
       </c>
       <c r="I245" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6483,14 +6488,14 @@
         <v>9</v>
       </c>
       <c r="G246" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H246" s="9">
         <v>0</v>
       </c>
       <c r="I246" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6505,14 +6510,14 @@
         <v>9</v>
       </c>
       <c r="G247" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H247" s="9">
         <v>0</v>
       </c>
       <c r="I247" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6527,14 +6532,14 @@
         <v>9</v>
       </c>
       <c r="G248" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H248" s="9">
         <v>0</v>
       </c>
       <c r="I248" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6549,14 +6554,14 @@
         <v>9</v>
       </c>
       <c r="G249" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H249" s="9">
         <v>0</v>
       </c>
       <c r="I249" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6571,14 +6576,14 @@
         <v>9</v>
       </c>
       <c r="G250" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H250" s="9">
         <v>0</v>
       </c>
       <c r="I250" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6593,14 +6598,14 @@
         <v>9</v>
       </c>
       <c r="G251" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H251" s="9">
         <v>0</v>
       </c>
       <c r="I251" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6615,14 +6620,14 @@
         <v>9</v>
       </c>
       <c r="G252" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H252" s="9">
         <v>0</v>
       </c>
       <c r="I252" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6637,14 +6642,14 @@
         <v>9</v>
       </c>
       <c r="G253" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H253" s="9">
         <v>0</v>
       </c>
       <c r="I253" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6659,14 +6664,14 @@
         <v>9</v>
       </c>
       <c r="G254" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H254" s="9">
         <v>0</v>
       </c>
       <c r="I254" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6681,14 +6686,14 @@
         <v>9</v>
       </c>
       <c r="G255" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H255" s="9">
         <v>0</v>
       </c>
       <c r="I255" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6703,14 +6708,14 @@
         <v>9</v>
       </c>
       <c r="G256" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H256" s="9">
         <v>0</v>
       </c>
       <c r="I256" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6725,14 +6730,14 @@
         <v>9</v>
       </c>
       <c r="G257" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H257" s="9">
         <v>0</v>
       </c>
       <c r="I257" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6747,14 +6752,14 @@
         <v>9</v>
       </c>
       <c r="G258" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H258" s="9">
         <v>0</v>
       </c>
       <c r="I258" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6769,14 +6774,14 @@
         <v>9</v>
       </c>
       <c r="G259" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H259" s="9">
         <v>0</v>
       </c>
       <c r="I259" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6791,14 +6796,14 @@
         <v>9</v>
       </c>
       <c r="G260" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H260" s="9">
         <v>0</v>
       </c>
       <c r="I260" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6813,14 +6818,14 @@
         <v>9</v>
       </c>
       <c r="G261" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H261" s="9">
         <v>0</v>
       </c>
       <c r="I261" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6835,14 +6840,14 @@
         <v>9</v>
       </c>
       <c r="G262" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H262" s="9">
         <v>0</v>
       </c>
       <c r="I262" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6857,14 +6862,14 @@
         <v>9</v>
       </c>
       <c r="G263" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H263" s="9">
         <v>0</v>
       </c>
       <c r="I263" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6879,14 +6884,14 @@
         <v>9</v>
       </c>
       <c r="G264" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H264" s="9">
         <v>0</v>
       </c>
       <c r="I264" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6901,14 +6906,14 @@
         <v>9</v>
       </c>
       <c r="G265" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H265" s="9">
         <v>0</v>
       </c>
       <c r="I265" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6923,14 +6928,14 @@
         <v>9</v>
       </c>
       <c r="G266" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H266" s="9">
         <v>0</v>
       </c>
       <c r="I266" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6945,14 +6950,14 @@
         <v>9</v>
       </c>
       <c r="G267" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H267" s="9">
         <v>0</v>
       </c>
       <c r="I267" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6967,14 +6972,14 @@
         <v>9</v>
       </c>
       <c r="G268" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H268" s="9">
         <v>0</v>
       </c>
       <c r="I268" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -6989,14 +6994,14 @@
         <v>9</v>
       </c>
       <c r="G269" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H269" s="9">
         <v>0</v>
       </c>
       <c r="I269" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7011,14 +7016,14 @@
         <v>9</v>
       </c>
       <c r="G270" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H270" s="9">
         <v>0</v>
       </c>
       <c r="I270" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7033,14 +7038,14 @@
         <v>9</v>
       </c>
       <c r="G271" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H271" s="9">
         <v>0</v>
       </c>
       <c r="I271" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7055,14 +7060,14 @@
         <v>9</v>
       </c>
       <c r="G272" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H272" s="9">
         <v>0</v>
       </c>
       <c r="I272" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7077,14 +7082,14 @@
         <v>9</v>
       </c>
       <c r="G273" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H273" s="9">
         <v>0</v>
       </c>
       <c r="I273" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7099,14 +7104,14 @@
         <v>9</v>
       </c>
       <c r="G274" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H274" s="9">
         <v>0</v>
       </c>
       <c r="I274" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7121,14 +7126,14 @@
         <v>9</v>
       </c>
       <c r="G275" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H275" s="9">
         <v>0</v>
       </c>
       <c r="I275" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7143,14 +7148,14 @@
         <v>9</v>
       </c>
       <c r="G276" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H276" s="9">
         <v>0</v>
       </c>
       <c r="I276" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7165,14 +7170,14 @@
         <v>9</v>
       </c>
       <c r="G277" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H277" s="9">
         <v>0</v>
       </c>
       <c r="I277" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7187,14 +7192,14 @@
         <v>9</v>
       </c>
       <c r="G278" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H278" s="9">
         <v>0</v>
       </c>
       <c r="I278" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7209,14 +7214,14 @@
         <v>9</v>
       </c>
       <c r="G279" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H279" s="9">
         <v>0</v>
       </c>
       <c r="I279" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7231,14 +7236,14 @@
         <v>9</v>
       </c>
       <c r="G280" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H280" s="9">
         <v>0</v>
       </c>
       <c r="I280" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7253,14 +7258,14 @@
         <v>9</v>
       </c>
       <c r="G281" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H281" s="9">
         <v>0</v>
       </c>
       <c r="I281" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7275,14 +7280,14 @@
         <v>9</v>
       </c>
       <c r="G282" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H282" s="9">
         <v>0</v>
       </c>
       <c r="I282" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7297,14 +7302,14 @@
         <v>9</v>
       </c>
       <c r="G283" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H283" s="9">
         <v>0</v>
       </c>
       <c r="I283" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7319,14 +7324,14 @@
         <v>9</v>
       </c>
       <c r="G284" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H284" s="9">
         <v>0</v>
       </c>
       <c r="I284" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7341,14 +7346,14 @@
         <v>9</v>
       </c>
       <c r="G285" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H285" s="9">
         <v>0</v>
       </c>
       <c r="I285" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7363,14 +7368,14 @@
         <v>9</v>
       </c>
       <c r="G286" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H286" s="9">
         <v>0</v>
       </c>
       <c r="I286" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7385,14 +7390,14 @@
         <v>9</v>
       </c>
       <c r="G287" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H287" s="9">
         <v>0</v>
       </c>
       <c r="I287" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7407,14 +7412,14 @@
         <v>9</v>
       </c>
       <c r="G288" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H288" s="9">
         <v>0</v>
       </c>
       <c r="I288" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7429,14 +7434,14 @@
         <v>9</v>
       </c>
       <c r="G289" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H289" s="9">
         <v>0</v>
       </c>
       <c r="I289" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7451,14 +7456,14 @@
         <v>9</v>
       </c>
       <c r="G290" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H290" s="9">
         <v>0</v>
       </c>
       <c r="I290" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7473,14 +7478,14 @@
         <v>9</v>
       </c>
       <c r="G291" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H291" s="9">
         <v>0</v>
       </c>
       <c r="I291" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7495,14 +7500,14 @@
         <v>9</v>
       </c>
       <c r="G292" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H292" s="9">
         <v>0</v>
       </c>
       <c r="I292" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7517,14 +7522,14 @@
         <v>9</v>
       </c>
       <c r="G293" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H293" s="9">
         <v>0</v>
       </c>
       <c r="I293" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7539,14 +7544,14 @@
         <v>9</v>
       </c>
       <c r="G294" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H294" s="9">
         <v>0</v>
       </c>
       <c r="I294" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7561,14 +7566,14 @@
         <v>9</v>
       </c>
       <c r="G295" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H295" s="9">
         <v>0</v>
       </c>
       <c r="I295" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7583,14 +7588,14 @@
         <v>9</v>
       </c>
       <c r="G296" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H296" s="9">
         <v>0</v>
       </c>
       <c r="I296" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7605,14 +7610,14 @@
         <v>9</v>
       </c>
       <c r="G297" s="25">
-        <f t="shared" ref="G297:G358" si="14">F297*D297</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H297" s="9">
         <v>0</v>
       </c>
       <c r="I297" s="25">
-        <f t="shared" ref="I297:I358" si="15">H297+G297</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7627,14 +7632,14 @@
         <v>9</v>
       </c>
       <c r="G298" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H298" s="9">
         <v>0</v>
       </c>
       <c r="I298" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7649,14 +7654,14 @@
         <v>9</v>
       </c>
       <c r="G299" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="H299" s="9">
         <v>0</v>
       </c>
       <c r="I299" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -7671,14 +7676,14 @@
         <v>9</v>
       </c>
       <c r="G300" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="G300:G361" si="20">F300*D300</f>
         <v>0</v>
       </c>
       <c r="H300" s="9">
         <v>0</v>
       </c>
       <c r="I300" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="I300:I361" si="21">H300+G300</f>
         <v>0</v>
       </c>
     </row>
@@ -7693,14 +7698,14 @@
         <v>9</v>
       </c>
       <c r="G301" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H301" s="9">
         <v>0</v>
       </c>
       <c r="I301" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7715,14 +7720,14 @@
         <v>9</v>
       </c>
       <c r="G302" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H302" s="9">
         <v>0</v>
       </c>
       <c r="I302" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7737,14 +7742,14 @@
         <v>9</v>
       </c>
       <c r="G303" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H303" s="9">
         <v>0</v>
       </c>
       <c r="I303" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7759,14 +7764,14 @@
         <v>9</v>
       </c>
       <c r="G304" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H304" s="9">
         <v>0</v>
       </c>
       <c r="I304" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7781,14 +7786,14 @@
         <v>9</v>
       </c>
       <c r="G305" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H305" s="9">
         <v>0</v>
       </c>
       <c r="I305" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7803,14 +7808,14 @@
         <v>9</v>
       </c>
       <c r="G306" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H306" s="9">
         <v>0</v>
       </c>
       <c r="I306" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7825,14 +7830,14 @@
         <v>9</v>
       </c>
       <c r="G307" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H307" s="9">
         <v>0</v>
       </c>
       <c r="I307" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7847,14 +7852,14 @@
         <v>9</v>
       </c>
       <c r="G308" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H308" s="9">
         <v>0</v>
       </c>
       <c r="I308" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7869,14 +7874,14 @@
         <v>9</v>
       </c>
       <c r="G309" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H309" s="9">
         <v>0</v>
       </c>
       <c r="I309" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7891,14 +7896,14 @@
         <v>9</v>
       </c>
       <c r="G310" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H310" s="9">
         <v>0</v>
       </c>
       <c r="I310" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7913,14 +7918,14 @@
         <v>9</v>
       </c>
       <c r="G311" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H311" s="9">
         <v>0</v>
       </c>
       <c r="I311" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7935,14 +7940,14 @@
         <v>9</v>
       </c>
       <c r="G312" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H312" s="9">
         <v>0</v>
       </c>
       <c r="I312" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7957,14 +7962,14 @@
         <v>9</v>
       </c>
       <c r="G313" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H313" s="9">
         <v>0</v>
       </c>
       <c r="I313" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7979,14 +7984,14 @@
         <v>9</v>
       </c>
       <c r="G314" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H314" s="9">
         <v>0</v>
       </c>
       <c r="I314" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8001,14 +8006,14 @@
         <v>9</v>
       </c>
       <c r="G315" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H315" s="9">
         <v>0</v>
       </c>
       <c r="I315" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8023,14 +8028,14 @@
         <v>9</v>
       </c>
       <c r="G316" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H316" s="9">
         <v>0</v>
       </c>
       <c r="I316" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8045,14 +8050,14 @@
         <v>9</v>
       </c>
       <c r="G317" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H317" s="9">
         <v>0</v>
       </c>
       <c r="I317" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8067,14 +8072,14 @@
         <v>9</v>
       </c>
       <c r="G318" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H318" s="9">
         <v>0</v>
       </c>
       <c r="I318" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8089,14 +8094,14 @@
         <v>9</v>
       </c>
       <c r="G319" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H319" s="9">
         <v>0</v>
       </c>
       <c r="I319" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8111,14 +8116,14 @@
         <v>9</v>
       </c>
       <c r="G320" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H320" s="9">
         <v>0</v>
       </c>
       <c r="I320" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8133,14 +8138,14 @@
         <v>9</v>
       </c>
       <c r="G321" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H321" s="9">
         <v>0</v>
       </c>
       <c r="I321" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8155,14 +8160,14 @@
         <v>9</v>
       </c>
       <c r="G322" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H322" s="9">
         <v>0</v>
       </c>
       <c r="I322" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8177,14 +8182,14 @@
         <v>9</v>
       </c>
       <c r="G323" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H323" s="9">
         <v>0</v>
       </c>
       <c r="I323" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8199,14 +8204,14 @@
         <v>9</v>
       </c>
       <c r="G324" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H324" s="9">
         <v>0</v>
       </c>
       <c r="I324" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8221,14 +8226,14 @@
         <v>9</v>
       </c>
       <c r="G325" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H325" s="9">
         <v>0</v>
       </c>
       <c r="I325" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8243,14 +8248,14 @@
         <v>9</v>
       </c>
       <c r="G326" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H326" s="9">
         <v>0</v>
       </c>
       <c r="I326" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8265,14 +8270,14 @@
         <v>9</v>
       </c>
       <c r="G327" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H327" s="9">
         <v>0</v>
       </c>
       <c r="I327" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8287,14 +8292,14 @@
         <v>9</v>
       </c>
       <c r="G328" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H328" s="9">
         <v>0</v>
       </c>
       <c r="I328" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8309,14 +8314,14 @@
         <v>9</v>
       </c>
       <c r="G329" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H329" s="9">
         <v>0</v>
       </c>
       <c r="I329" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8331,14 +8336,14 @@
         <v>9</v>
       </c>
       <c r="G330" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H330" s="9">
         <v>0</v>
       </c>
       <c r="I330" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8353,14 +8358,14 @@
         <v>9</v>
       </c>
       <c r="G331" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H331" s="9">
         <v>0</v>
       </c>
       <c r="I331" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8375,14 +8380,14 @@
         <v>9</v>
       </c>
       <c r="G332" s="25">
-        <f t="shared" ref="G332" si="16">F332*D332</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H332" s="9">
         <v>0</v>
       </c>
       <c r="I332" s="25">
-        <f t="shared" ref="I332" si="17">H332+G332</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8397,14 +8402,14 @@
         <v>9</v>
       </c>
       <c r="G333" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H333" s="9">
         <v>0</v>
       </c>
       <c r="I333" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8419,14 +8424,14 @@
         <v>9</v>
       </c>
       <c r="G334" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H334" s="9">
         <v>0</v>
       </c>
       <c r="I334" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8441,14 +8446,14 @@
         <v>9</v>
       </c>
       <c r="G335" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H335" s="9">
         <v>0</v>
       </c>
       <c r="I335" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8463,14 +8468,14 @@
         <v>9</v>
       </c>
       <c r="G336" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H336" s="9">
         <v>0</v>
       </c>
       <c r="I336" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8485,14 +8490,14 @@
         <v>9</v>
       </c>
       <c r="G337" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H337" s="9">
         <v>0</v>
       </c>
       <c r="I337" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8507,14 +8512,14 @@
         <v>9</v>
       </c>
       <c r="G338" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H338" s="9">
         <v>0</v>
       </c>
       <c r="I338" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8529,14 +8534,14 @@
         <v>9</v>
       </c>
       <c r="G339" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H339" s="9">
         <v>0</v>
       </c>
       <c r="I339" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8551,14 +8556,14 @@
         <v>9</v>
       </c>
       <c r="G340" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H340" s="9">
         <v>0</v>
       </c>
       <c r="I340" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8573,14 +8578,14 @@
         <v>9</v>
       </c>
       <c r="G341" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H341" s="9">
         <v>0</v>
       </c>
       <c r="I341" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8595,14 +8600,14 @@
         <v>9</v>
       </c>
       <c r="G342" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H342" s="9">
         <v>0</v>
       </c>
       <c r="I342" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8617,14 +8622,14 @@
         <v>9</v>
       </c>
       <c r="G343" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H343" s="9">
         <v>0</v>
       </c>
       <c r="I343" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8639,14 +8644,14 @@
         <v>9</v>
       </c>
       <c r="G344" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H344" s="9">
         <v>0</v>
       </c>
       <c r="I344" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8661,14 +8666,14 @@
         <v>9</v>
       </c>
       <c r="G345" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H345" s="9">
         <v>0</v>
       </c>
       <c r="I345" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8683,14 +8688,14 @@
         <v>9</v>
       </c>
       <c r="G346" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H346" s="9">
         <v>0</v>
       </c>
       <c r="I346" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8705,14 +8710,14 @@
         <v>9</v>
       </c>
       <c r="G347" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H347" s="9">
         <v>0</v>
       </c>
       <c r="I347" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8727,14 +8732,14 @@
         <v>9</v>
       </c>
       <c r="G348" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H348" s="9">
         <v>0</v>
       </c>
       <c r="I348" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8749,14 +8754,14 @@
         <v>9</v>
       </c>
       <c r="G349" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H349" s="9">
         <v>0</v>
       </c>
       <c r="I349" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8771,14 +8776,14 @@
         <v>9</v>
       </c>
       <c r="G350" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H350" s="9">
         <v>0</v>
       </c>
       <c r="I350" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8793,14 +8798,14 @@
         <v>9</v>
       </c>
       <c r="G351" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H351" s="9">
         <v>0</v>
       </c>
       <c r="I351" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8815,14 +8820,14 @@
         <v>9</v>
       </c>
       <c r="G352" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H352" s="9">
         <v>0</v>
       </c>
       <c r="I352" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8837,14 +8842,14 @@
         <v>9</v>
       </c>
       <c r="G353" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H353" s="9">
         <v>0</v>
       </c>
       <c r="I353" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8859,14 +8864,14 @@
         <v>9</v>
       </c>
       <c r="G354" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H354" s="9">
         <v>0</v>
       </c>
       <c r="I354" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8881,14 +8886,14 @@
         <v>9</v>
       </c>
       <c r="G355" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H355" s="9">
         <v>0</v>
       </c>
       <c r="I355" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8903,14 +8908,14 @@
         <v>9</v>
       </c>
       <c r="G356" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H356" s="9">
         <v>0</v>
       </c>
       <c r="I356" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8925,14 +8930,14 @@
         <v>9</v>
       </c>
       <c r="G357" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H357" s="9">
         <v>0</v>
       </c>
       <c r="I357" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8947,14 +8952,14 @@
         <v>9</v>
       </c>
       <c r="G358" s="25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H358" s="9">
         <v>0</v>
       </c>
       <c r="I358" s="25">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8969,14 +8974,14 @@
         <v>9</v>
       </c>
       <c r="G359" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H359" s="9">
         <v>0</v>
       </c>
       <c r="I359" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -8992,14 +8997,14 @@
       </c>
       <c r="F360"/>
       <c r="G360" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H360" s="9">
         <v>0</v>
       </c>
       <c r="I360" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -9015,14 +9020,14 @@
       </c>
       <c r="F361"/>
       <c r="G361" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H361" s="9">
         <v>0</v>
       </c>
       <c r="I361" s="25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -9092,14 +9097,14 @@
         <v>9</v>
       </c>
       <c r="G367" s="25">
-        <f t="shared" ref="G367:G371" si="18">F367*D367</f>
+        <f t="shared" ref="G367:G371" si="22">F367*D367</f>
         <v>0</v>
       </c>
       <c r="H367" s="9">
         <v>0</v>
       </c>
       <c r="I367" s="25">
-        <f t="shared" ref="I367:I371" si="19">H367+G367</f>
+        <f t="shared" ref="I367:I371" si="23">H367+G367</f>
         <v>0</v>
       </c>
     </row>
@@ -9115,14 +9120,14 @@
       </c>
       <c r="F368"/>
       <c r="G368" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H368" s="9">
         <v>0</v>
       </c>
       <c r="I368" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="J368"/>
@@ -9138,14 +9143,14 @@
         <v>9</v>
       </c>
       <c r="G369" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H369" s="9">
         <v>0</v>
       </c>
       <c r="I369" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -9160,14 +9165,14 @@
         <v>9</v>
       </c>
       <c r="G370" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H370" s="9">
         <v>0</v>
       </c>
       <c r="I370" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -9182,14 +9187,14 @@
         <v>9</v>
       </c>
       <c r="G371" s="25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="H371" s="9">
         <v>0</v>
       </c>
       <c r="I371" s="25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
     </row>
@@ -9314,14 +9319,14 @@
         <v>9</v>
       </c>
       <c r="G380" s="25">
-        <f t="shared" ref="G380:G381" si="20">D380*F380</f>
+        <f t="shared" ref="G380:G381" si="24">D380*F380</f>
         <v>0</v>
       </c>
       <c r="H380" s="9">
         <v>0</v>
       </c>
       <c r="I380" s="25">
-        <f t="shared" ref="I380:I381" si="21">G380+H380</f>
+        <f t="shared" ref="I380:I381" si="25">G380+H380</f>
         <v>0</v>
       </c>
     </row>
@@ -9334,14 +9339,14 @@
         <v>9</v>
       </c>
       <c r="G381" s="25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="H381" s="9">
         <v>0</v>
       </c>
       <c r="I381" s="25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
     </row>
@@ -9432,14 +9437,14 @@
       </c>
       <c r="F391" s="54"/>
       <c r="G391" s="55">
-        <f t="shared" ref="G391:G403" si="22">F391*D391</f>
+        <f t="shared" ref="G391:G403" si="26">F391*D391</f>
         <v>0</v>
       </c>
       <c r="H391" s="56">
         <v>0</v>
       </c>
       <c r="I391" s="55">
-        <f t="shared" ref="I391:I403" si="23">H391+G391</f>
+        <f t="shared" ref="I391:I403" si="27">H391+G391</f>
         <v>0</v>
       </c>
     </row>
@@ -9452,14 +9457,14 @@
         <v>20</v>
       </c>
       <c r="G392" s="25">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="H392" s="48">
         <v>0</v>
       </c>
       <c r="I392" s="25">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -9475,14 +9480,14 @@
       </c>
       <c r="F393" s="82"/>
       <c r="G393" s="84">
-        <f t="shared" ref="G393:G401" si="24">F393*D393</f>
+        <f t="shared" ref="G393:G401" si="28">F393*D393</f>
         <v>0</v>
       </c>
       <c r="H393" s="83">
         <v>0</v>
       </c>
       <c r="I393" s="84">
-        <f t="shared" ref="I393:I401" si="25">H393+G393</f>
+        <f t="shared" ref="I393:I401" si="29">H393+G393</f>
         <v>0</v>
       </c>
     </row>
@@ -9498,14 +9503,14 @@
       </c>
       <c r="F394" s="82"/>
       <c r="G394" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H394" s="83">
         <v>0</v>
       </c>
       <c r="I394" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9521,14 +9526,14 @@
       </c>
       <c r="F395" s="82"/>
       <c r="G395" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H395" s="83">
         <v>0</v>
       </c>
       <c r="I395" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9544,14 +9549,14 @@
       </c>
       <c r="F396" s="82"/>
       <c r="G396" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H396" s="83">
         <v>0</v>
       </c>
       <c r="I396" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9567,14 +9572,14 @@
       </c>
       <c r="F397" s="82"/>
       <c r="G397" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H397" s="83">
         <v>0</v>
       </c>
       <c r="I397" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9587,14 +9592,14 @@
         <v>20</v>
       </c>
       <c r="G398" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H398" s="83">
         <v>0</v>
       </c>
       <c r="I398" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9607,14 +9612,14 @@
         <v>20</v>
       </c>
       <c r="G399" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H399" s="83">
         <v>0</v>
       </c>
       <c r="I399" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9627,14 +9632,14 @@
         <v>20</v>
       </c>
       <c r="G400" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H400" s="83">
         <v>0</v>
       </c>
       <c r="I400" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9647,14 +9652,14 @@
         <v>20</v>
       </c>
       <c r="G401" s="84">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="H401" s="83">
         <v>0</v>
       </c>
       <c r="I401" s="84">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
     </row>
@@ -9667,14 +9672,14 @@
         <v>20</v>
       </c>
       <c r="G402" s="84">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="H402" s="83">
         <v>0</v>
       </c>
       <c r="I402" s="84">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -9689,14 +9694,14 @@
         <v>20</v>
       </c>
       <c r="G403" s="84">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="H403" s="83">
         <v>0</v>
       </c>
       <c r="I403" s="84">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -9776,14 +9781,14 @@
       </c>
       <c r="F411" s="54"/>
       <c r="G411" s="55">
-        <f t="shared" ref="G411" si="26">F411*D411</f>
+        <f t="shared" ref="G411" si="30">F411*D411</f>
         <v>0</v>
       </c>
       <c r="H411" s="56">
         <v>0</v>
       </c>
       <c r="I411" s="55">
-        <f t="shared" ref="I411" si="27">H411+G411</f>
+        <f t="shared" ref="I411" si="31">H411+G411</f>
         <v>0</v>
       </c>
     </row>
@@ -10119,39 +10124,29 @@
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="E107 E359:E361">
-    <cfRule type="containsErrors" dxfId="6" priority="10">
+  <conditionalFormatting sqref="E107">
+    <cfRule type="containsErrors" dxfId="10" priority="12">
       <formula>ISERROR(E107)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E367:E371">
-    <cfRule type="containsErrors" dxfId="5" priority="8">
+    <cfRule type="containsErrors" dxfId="9" priority="10">
       <formula>ISERROR(E367)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E377:E381">
-    <cfRule type="containsErrors" dxfId="4" priority="7">
+    <cfRule type="containsErrors" dxfId="8" priority="9">
       <formula>ISERROR(E377)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="containsErrors" dxfId="3" priority="4">
+    <cfRule type="containsErrors" dxfId="7" priority="6">
       <formula>ISERROR(E106)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E297:E331 E333:E358">
-    <cfRule type="containsErrors" dxfId="2" priority="3">
-      <formula>ISERROR(E297)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108:E296">
-    <cfRule type="containsErrors" dxfId="1" priority="2">
+  <conditionalFormatting sqref="E108:E361">
+    <cfRule type="containsErrors" dxfId="1" priority="1">
       <formula>ISERROR(E108)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E332">
-    <cfRule type="containsErrors" dxfId="0" priority="1">
-      <formula>ISERROR(E332)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added Canvas to Labor Rates At Bottom of Sheet
</commit_message>
<xml_diff>
--- a/CostingSheetTemplate.xlsx
+++ b/CostingSheetTemplate.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="56">
   <si>
     <t>Boat #</t>
   </si>
@@ -916,49 +916,7 @@
     <cellStyle name="Total" xfId="41" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="42" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -3430,14 +3388,14 @@
         <v>9</v>
       </c>
       <c r="G107" s="25">
-        <f t="shared" ref="G107:G361" si="12">F107*D107</f>
+        <f t="shared" ref="G107" si="12">F107*D107</f>
         <v>0</v>
       </c>
       <c r="H107" s="9">
         <v>0</v>
       </c>
       <c r="I107" s="25">
-        <f t="shared" ref="I107:I361" si="13">H107+G107</f>
+        <f t="shared" ref="I107" si="13">H107+G107</f>
         <v>0</v>
       </c>
     </row>
@@ -9929,10 +9887,17 @@
       </c>
     </row>
     <row r="430" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D430" s="34"/>
+      <c r="D430" s="34" t="s">
+        <v>54</v>
+      </c>
       <c r="F430" s="14"/>
-      <c r="G430" s="44"/>
-      <c r="I430" s="25"/>
+      <c r="G430" s="44">
+        <v>35.619999999999997</v>
+      </c>
+      <c r="I430" s="25">
+        <f>G430*F430</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="431" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D431" s="34" t="s">
@@ -9960,7 +9925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="433" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="433" spans="3:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D433" s="34" t="s">
         <v>34</v>
       </c>
@@ -10125,27 +10090,27 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="E107">
-    <cfRule type="containsErrors" dxfId="10" priority="12">
+    <cfRule type="containsErrors" dxfId="4" priority="12">
       <formula>ISERROR(E107)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E367:E371">
-    <cfRule type="containsErrors" dxfId="9" priority="10">
+    <cfRule type="containsErrors" dxfId="3" priority="10">
       <formula>ISERROR(E367)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E377:E381">
-    <cfRule type="containsErrors" dxfId="8" priority="9">
+    <cfRule type="containsErrors" dxfId="2" priority="9">
       <formula>ISERROR(E377)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="containsErrors" dxfId="7" priority="6">
+    <cfRule type="containsErrors" dxfId="1" priority="6">
       <formula>ISERROR(E106)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108:E361">
-    <cfRule type="containsErrors" dxfId="1" priority="1">
+    <cfRule type="containsErrors" dxfId="0" priority="1">
       <formula>ISERROR(E108)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated template and processing logic
- Added 'Canvas' to Labor Section
- Changed 'Engine - Jet' to 'Engine & Jet' in Materials
- Process 'Engine & Jet' in Materials Section
</commit_message>
<xml_diff>
--- a/CostingSheetTemplate.xlsx
+++ b/CostingSheetTemplate.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\costing-sheets-rec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B0A513-39E7-40FD-A7CF-768BE9A005DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22935" yWindow="-105" windowWidth="23250" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="COSTING SHEET" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'COSTING SHEET'!$A$2:$I$421</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="55">
   <si>
     <t>Boat #</t>
   </si>
@@ -186,9 +185,6 @@
     <t xml:space="preserve">TOTAL ENGINE &amp; JET </t>
   </si>
   <si>
-    <t>Engine - Jet</t>
-  </si>
-  <si>
     <t>Canvas Materials</t>
   </si>
   <si>
@@ -204,7 +200,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -874,7 +870,7 @@
     <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="27" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Currency" xfId="28" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Currency 2" xfId="43"/>
     <cellStyle name="Explanatory Text" xfId="29" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="30" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="31" builtinId="16" customBuiltin="1"/>
@@ -1030,23 +1026,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1082,23 +1061,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1274,26 +1236,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J461"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="4.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="28.2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
       <c r="C2" s="24">
@@ -1302,7 +1264,7 @@
       <c r="D2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="28.2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
@@ -1311,16 +1273,16 @@
       <c r="D3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B4" s="34"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C5" s="64" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="55" t="s">
         <v>2</v>
       </c>
@@ -1345,7 +1307,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="65"/>
       <c r="B8" s="66"/>
       <c r="C8" s="66"/>
@@ -1367,7 +1329,7 @@
       </c>
       <c r="J8" s="23"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="38"/>
@@ -1389,7 +1351,7 @@
       </c>
       <c r="J9" s="23"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="38"/>
@@ -1411,7 +1373,7 @@
       </c>
       <c r="J10" s="23"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="38"/>
@@ -1433,7 +1395,7 @@
       </c>
       <c r="J11" s="23"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="38"/>
@@ -1455,7 +1417,7 @@
       </c>
       <c r="J12" s="23"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="38"/>
@@ -1477,7 +1439,7 @@
       </c>
       <c r="J13" s="23"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="38"/>
@@ -1499,7 +1461,7 @@
       </c>
       <c r="J14" s="23"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="38"/>
@@ -1521,7 +1483,7 @@
       </c>
       <c r="J15" s="23"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="38"/>
@@ -1543,7 +1505,7 @@
       </c>
       <c r="J16" s="23"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="38"/>
@@ -1565,7 +1527,7 @@
       </c>
       <c r="J17" s="23"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="38"/>
@@ -1587,7 +1549,7 @@
       </c>
       <c r="J18" s="23"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="38"/>
@@ -1609,7 +1571,7 @@
       </c>
       <c r="J19" s="23"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="38"/>
@@ -1631,7 +1593,7 @@
       </c>
       <c r="J20" s="23"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="38"/>
@@ -1653,7 +1615,7 @@
       </c>
       <c r="J21" s="23"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="38"/>
@@ -1675,7 +1637,7 @@
       </c>
       <c r="J22" s="23"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="38"/>
@@ -1697,7 +1659,7 @@
       </c>
       <c r="J23" s="23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" s="16"/>
       <c r="C24" s="38"/>
@@ -1719,7 +1681,7 @@
       </c>
       <c r="J24" s="23"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
       <c r="B25" s="16"/>
       <c r="C25" s="38"/>
@@ -1741,7 +1703,7 @@
       </c>
       <c r="J25" s="23"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
       <c r="B26" s="16"/>
       <c r="C26" s="38"/>
@@ -1763,7 +1725,7 @@
       </c>
       <c r="J26" s="23"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="38"/>
@@ -1785,7 +1747,7 @@
       </c>
       <c r="J27" s="23"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="38"/>
@@ -1807,7 +1769,7 @@
       </c>
       <c r="J28" s="23"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
       <c r="B29" s="16"/>
       <c r="C29" s="38"/>
@@ -1829,7 +1791,7 @@
       </c>
       <c r="J29" s="23"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="16"/>
       <c r="C30" s="38"/>
@@ -1851,7 +1813,7 @@
       </c>
       <c r="J30" s="23"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="16"/>
       <c r="C31" s="38"/>
@@ -1873,7 +1835,7 @@
       </c>
       <c r="J31" s="23"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="38"/>
@@ -1895,7 +1857,7 @@
       </c>
       <c r="J32" s="23"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="38"/>
@@ -1917,7 +1879,7 @@
       </c>
       <c r="J33" s="23"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="38"/>
@@ -1939,7 +1901,7 @@
       </c>
       <c r="J34" s="23"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C35" s="14"/>
       <c r="H35" s="13" t="s">
         <v>46</v>
@@ -1950,7 +1912,7 @@
       </c>
       <c r="J35" s="23"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C36" s="14"/>
       <c r="H36" s="13" t="s">
         <v>10</v>
@@ -1961,7 +1923,7 @@
       </c>
       <c r="J36" s="23"/>
     </row>
-    <row r="37" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -1973,12 +1935,12 @@
       <c r="I37" s="17"/>
       <c r="J37" s="23"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H38" s="13"/>
       <c r="I38" s="15"/>
       <c r="J38" s="23"/>
     </row>
-    <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1989,12 +1951,12 @@
       <c r="I39" s="15"/>
       <c r="J39" s="23"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H40" s="13"/>
       <c r="I40" s="15"/>
       <c r="J40" s="22"/>
     </row>
-    <row r="41" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="55" t="s">
         <v>2</v>
       </c>
@@ -2021,7 +1983,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="66"/>
       <c r="B42" s="66"/>
       <c r="C42" s="70"/>
@@ -2045,7 +2007,7 @@
       </c>
       <c r="J42" s="23"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="16"/>
       <c r="B43" s="16"/>
       <c r="C43" s="38"/>
@@ -2069,7 +2031,7 @@
       </c>
       <c r="J43" s="23"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="16"/>
       <c r="B44" s="16"/>
       <c r="C44" s="38"/>
@@ -2093,7 +2055,7 @@
       </c>
       <c r="J44" s="23"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="16"/>
       <c r="C45" s="38"/>
@@ -2117,7 +2079,7 @@
       </c>
       <c r="J45" s="23"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="38"/>
@@ -2141,7 +2103,7 @@
       </c>
       <c r="J46" s="23"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="16"/>
       <c r="C47" s="38"/>
@@ -2165,7 +2127,7 @@
       </c>
       <c r="J47" s="23"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="16"/>
       <c r="C48" s="38"/>
@@ -2189,7 +2151,7 @@
       </c>
       <c r="J48" s="23"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="16"/>
       <c r="C49" s="38"/>
@@ -2213,7 +2175,7 @@
       </c>
       <c r="J49" s="23"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="16"/>
       <c r="B50" s="16"/>
       <c r="C50" s="38"/>
@@ -2237,7 +2199,7 @@
       </c>
       <c r="J50" s="23"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="16"/>
       <c r="B51" s="16"/>
       <c r="C51" s="38"/>
@@ -2261,7 +2223,7 @@
       </c>
       <c r="J51" s="23"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="16"/>
       <c r="B52" s="16"/>
       <c r="C52" s="38"/>
@@ -2285,7 +2247,7 @@
       </c>
       <c r="J52" s="23"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="16"/>
       <c r="B53" s="16"/>
       <c r="C53" s="38"/>
@@ -2309,7 +2271,7 @@
       </c>
       <c r="J53" s="23"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
       <c r="B54" s="16"/>
       <c r="C54" s="38"/>
@@ -2333,7 +2295,7 @@
       </c>
       <c r="J54" s="23"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="16"/>
       <c r="B55" s="16"/>
       <c r="C55" s="38"/>
@@ -2357,7 +2319,7 @@
       </c>
       <c r="J55" s="23"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="16"/>
       <c r="C56" s="38"/>
@@ -2381,7 +2343,7 @@
       </c>
       <c r="J56" s="23"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
       <c r="B57" s="16"/>
       <c r="C57" s="38"/>
@@ -2405,7 +2367,7 @@
       </c>
       <c r="J57" s="23"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="16"/>
       <c r="B58" s="16"/>
       <c r="C58" s="38"/>
@@ -2429,7 +2391,7 @@
       </c>
       <c r="J58" s="23"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="16"/>
       <c r="B59" s="16"/>
       <c r="C59" s="38"/>
@@ -2453,7 +2415,7 @@
       </c>
       <c r="J59" s="23"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="16"/>
       <c r="B60" s="16"/>
       <c r="C60" s="38"/>
@@ -2477,7 +2439,7 @@
       </c>
       <c r="J60" s="23"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="16"/>
       <c r="B61" s="16"/>
       <c r="C61" s="38"/>
@@ -2501,7 +2463,7 @@
       </c>
       <c r="J61" s="23"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
       <c r="B62" s="16"/>
       <c r="C62" s="38"/>
@@ -2525,7 +2487,7 @@
       </c>
       <c r="J62" s="23"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
       <c r="B63" s="16"/>
       <c r="C63" s="38"/>
@@ -2549,7 +2511,7 @@
       </c>
       <c r="J63" s="23"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="16"/>
       <c r="C64" s="38"/>
@@ -2573,7 +2535,7 @@
       </c>
       <c r="J64" s="23"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="16"/>
       <c r="B65" s="16"/>
       <c r="C65" s="38"/>
@@ -2597,7 +2559,7 @@
       </c>
       <c r="J65" s="23"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
       <c r="B66" s="16"/>
       <c r="C66" s="38"/>
@@ -2621,7 +2583,7 @@
       </c>
       <c r="J66" s="23"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C67" s="14"/>
       <c r="H67" s="13" t="s">
         <v>46</v>
@@ -2632,7 +2594,7 @@
       </c>
       <c r="J67" s="23"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C68" s="14"/>
       <c r="H68" s="13" t="s">
         <v>13</v>
@@ -2643,7 +2605,7 @@
       </c>
       <c r="J68" s="23"/>
     </row>
-    <row r="69" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
@@ -2655,28 +2617,28 @@
       <c r="I69" s="12"/>
       <c r="J69" s="23"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H70" s="13"/>
       <c r="I70" s="15"/>
       <c r="J70" s="23"/>
     </row>
-    <row r="71" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H71" s="13"/>
       <c r="I71" s="15"/>
       <c r="J71" s="23"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="H72" s="13"/>
       <c r="I72" s="15"/>
       <c r="J72" s="22"/>
     </row>
-    <row r="73" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="55" t="s">
         <v>2</v>
       </c>
@@ -2703,7 +2665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="66"/>
       <c r="B74" s="66"/>
       <c r="C74" s="70"/>
@@ -2727,7 +2689,7 @@
       </c>
       <c r="J74" s="23"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
       <c r="B75" s="16"/>
       <c r="C75" s="38"/>
@@ -2751,7 +2713,7 @@
       </c>
       <c r="J75" s="23"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="16"/>
       <c r="B76" s="16"/>
       <c r="C76" s="38"/>
@@ -2775,7 +2737,7 @@
       </c>
       <c r="J76" s="23"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="16"/>
       <c r="B77" s="16"/>
       <c r="C77" s="38"/>
@@ -2799,7 +2761,7 @@
       </c>
       <c r="J77" s="23"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="16"/>
       <c r="B78" s="16"/>
       <c r="C78" s="38"/>
@@ -2823,7 +2785,7 @@
       </c>
       <c r="J78" s="23"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="16"/>
       <c r="B79" s="16"/>
       <c r="C79" s="38"/>
@@ -2847,7 +2809,7 @@
       </c>
       <c r="J79" s="23"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="16"/>
       <c r="C80" s="38"/>
@@ -2871,7 +2833,7 @@
       </c>
       <c r="J80" s="23"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="16"/>
       <c r="B81" s="16"/>
       <c r="C81" s="38"/>
@@ -2895,7 +2857,7 @@
       </c>
       <c r="J81" s="23"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="16"/>
       <c r="B82" s="16"/>
       <c r="C82" s="38"/>
@@ -2919,7 +2881,7 @@
       </c>
       <c r="J82" s="23"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="16"/>
       <c r="B83" s="16"/>
       <c r="C83" s="38"/>
@@ -2943,7 +2905,7 @@
       </c>
       <c r="J83" s="23"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="16"/>
       <c r="C84" s="38"/>
@@ -2967,7 +2929,7 @@
       </c>
       <c r="J84" s="23"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="16"/>
       <c r="B85" s="16"/>
       <c r="C85" s="38"/>
@@ -2991,7 +2953,7 @@
       </c>
       <c r="J85" s="23"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="16"/>
       <c r="B86" s="16"/>
       <c r="C86" s="38"/>
@@ -3015,7 +2977,7 @@
       </c>
       <c r="J86" s="23"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
       <c r="B87" s="16"/>
       <c r="C87" s="38"/>
@@ -3039,7 +3001,7 @@
       </c>
       <c r="J87" s="23"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
       <c r="B88" s="16"/>
       <c r="C88" s="38"/>
@@ -3063,7 +3025,7 @@
       </c>
       <c r="J88" s="23"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="16"/>
       <c r="B89" s="16"/>
       <c r="C89" s="38"/>
@@ -3087,7 +3049,7 @@
       </c>
       <c r="J89" s="23"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="16"/>
       <c r="B90" s="16"/>
       <c r="C90" s="38"/>
@@ -3111,7 +3073,7 @@
       </c>
       <c r="J90" s="23"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="16"/>
       <c r="B91" s="16"/>
       <c r="C91" s="38"/>
@@ -3135,7 +3097,7 @@
       </c>
       <c r="J91" s="23"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="16"/>
       <c r="B92" s="16"/>
       <c r="C92" s="38"/>
@@ -3159,7 +3121,7 @@
       </c>
       <c r="J92" s="23"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="16"/>
       <c r="B93" s="16"/>
       <c r="C93" s="38"/>
@@ -3183,7 +3145,7 @@
       </c>
       <c r="J93" s="23"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="16"/>
       <c r="B94" s="16"/>
       <c r="C94" s="38"/>
@@ -3207,7 +3169,7 @@
       </c>
       <c r="J94" s="23"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="16"/>
       <c r="B95" s="16"/>
       <c r="C95" s="38"/>
@@ -3231,7 +3193,7 @@
       </c>
       <c r="J95" s="23"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="16"/>
       <c r="B96" s="16"/>
       <c r="C96" s="38"/>
@@ -3255,7 +3217,7 @@
       </c>
       <c r="J96" s="23"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="16"/>
       <c r="B97" s="16"/>
       <c r="C97" s="38"/>
@@ -3279,7 +3241,7 @@
       </c>
       <c r="J97" s="23"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="16"/>
       <c r="B98" s="16"/>
       <c r="C98" s="38"/>
@@ -3303,7 +3265,7 @@
       </c>
       <c r="J98" s="23"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="23"/>
       <c r="B99" s="23"/>
       <c r="C99" s="49"/>
@@ -3315,10 +3277,10 @@
       <c r="I99" s="50"/>
       <c r="J99" s="23"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C100" s="14"/>
       <c r="H100" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I100" s="54">
         <f>SUM(I74:I98)</f>
@@ -3326,7 +3288,7 @@
       </c>
       <c r="J100" s="23"/>
     </row>
-    <row r="101" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
       <c r="B101" s="12"/>
       <c r="C101" s="12"/>
@@ -3338,18 +3300,18 @@
       <c r="I101" s="12"/>
       <c r="J101" s="23"/>
     </row>
-    <row r="103" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C103" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C104" s="3"/>
       <c r="D104" s="1"/>
       <c r="G104" s="2"/>
       <c r="H104" s="1"/>
     </row>
-    <row r="105" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A105" s="55" t="s">
         <v>2</v>
       </c>
@@ -3378,7 +3340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="72"/>
       <c r="B106" s="72"/>
       <c r="C106" s="72"/>
@@ -3401,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="19"/>
       <c r="B107" s="19"/>
       <c r="C107" s="19"/>
@@ -3423,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="19"/>
       <c r="B108" s="19"/>
       <c r="C108" s="19"/>
@@ -3445,7 +3407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="19"/>
       <c r="B109" s="19"/>
       <c r="C109" s="19"/>
@@ -3467,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="19"/>
       <c r="B110" s="19"/>
       <c r="C110" s="19"/>
@@ -3489,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="19"/>
       <c r="B111" s="19"/>
       <c r="C111" s="19"/>
@@ -3511,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="19"/>
       <c r="B112" s="19"/>
       <c r="C112" s="19"/>
@@ -3533,7 +3495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="19"/>
       <c r="B113" s="19"/>
       <c r="C113" s="19"/>
@@ -3555,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="19"/>
       <c r="B114" s="19"/>
       <c r="C114" s="19"/>
@@ -3577,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="19"/>
       <c r="B115" s="19"/>
       <c r="C115" s="19"/>
@@ -3599,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="19"/>
       <c r="B116" s="19"/>
       <c r="C116" s="19"/>
@@ -3621,7 +3583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="19"/>
       <c r="B117" s="19"/>
       <c r="C117" s="19"/>
@@ -3643,7 +3605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="19"/>
       <c r="B118" s="19"/>
       <c r="C118" s="19"/>
@@ -3665,7 +3627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="19"/>
       <c r="B119" s="19"/>
       <c r="C119" s="19"/>
@@ -3687,7 +3649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="19"/>
       <c r="B120" s="19"/>
       <c r="C120" s="19"/>
@@ -3709,7 +3671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="19"/>
       <c r="B121" s="19"/>
       <c r="C121" s="19"/>
@@ -3731,7 +3693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="19"/>
       <c r="B122" s="19"/>
       <c r="C122" s="19"/>
@@ -3753,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="19"/>
       <c r="B123" s="19"/>
       <c r="C123" s="19"/>
@@ -3775,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="19"/>
       <c r="B124" s="19"/>
       <c r="C124" s="19"/>
@@ -3797,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="19"/>
       <c r="B125" s="19"/>
       <c r="C125" s="19"/>
@@ -3819,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="19"/>
       <c r="B126" s="19"/>
       <c r="C126" s="19"/>
@@ -3841,7 +3803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="19"/>
       <c r="B127" s="19"/>
       <c r="C127" s="19"/>
@@ -3863,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="19"/>
       <c r="B128" s="19"/>
       <c r="C128" s="19"/>
@@ -3885,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" s="19"/>
       <c r="B129" s="19"/>
       <c r="C129" s="19"/>
@@ -3907,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" s="19"/>
       <c r="B130" s="19"/>
       <c r="C130" s="19"/>
@@ -3929,7 +3891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" s="19"/>
       <c r="B131" s="19"/>
       <c r="C131" s="19"/>
@@ -3951,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" s="19"/>
       <c r="B132" s="19"/>
       <c r="C132" s="19"/>
@@ -3973,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" s="19"/>
       <c r="B133" s="19"/>
       <c r="C133" s="19"/>
@@ -3995,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" s="19"/>
       <c r="B134" s="19"/>
       <c r="C134" s="19"/>
@@ -4017,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" s="19"/>
       <c r="B135" s="19"/>
       <c r="C135" s="19"/>
@@ -4039,7 +4001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" s="19"/>
       <c r="B136" s="19"/>
       <c r="C136" s="19"/>
@@ -4061,7 +4023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" s="19"/>
       <c r="B137" s="19"/>
       <c r="C137" s="19"/>
@@ -4083,7 +4045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" s="19"/>
       <c r="B138" s="19"/>
       <c r="C138" s="19"/>
@@ -4105,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" s="19"/>
       <c r="B139" s="19"/>
       <c r="C139" s="19"/>
@@ -4127,7 +4089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" s="19"/>
       <c r="B140" s="19"/>
       <c r="C140" s="19"/>
@@ -4149,7 +4111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" s="19"/>
       <c r="B141" s="19"/>
       <c r="C141" s="19"/>
@@ -4171,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" s="19"/>
       <c r="B142" s="19"/>
       <c r="C142" s="19"/>
@@ -4193,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" s="19"/>
       <c r="B143" s="19"/>
       <c r="C143" s="19"/>
@@ -4215,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" s="19"/>
       <c r="B144" s="19"/>
       <c r="C144" s="19"/>
@@ -4237,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" s="19"/>
       <c r="B145" s="19"/>
       <c r="C145" s="19"/>
@@ -4259,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" s="19"/>
       <c r="B146" s="19"/>
       <c r="C146" s="19"/>
@@ -4281,7 +4243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" s="19"/>
       <c r="B147" s="19"/>
       <c r="C147" s="19"/>
@@ -4303,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" s="19"/>
       <c r="B148" s="19"/>
       <c r="C148" s="19"/>
@@ -4325,7 +4287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" s="19"/>
       <c r="B149" s="19"/>
       <c r="C149" s="19"/>
@@ -4347,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" s="19"/>
       <c r="B150" s="19"/>
       <c r="C150" s="19"/>
@@ -4369,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" s="19"/>
       <c r="B151" s="19"/>
       <c r="C151" s="19"/>
@@ -4391,7 +4353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" s="19"/>
       <c r="B152" s="19"/>
       <c r="C152" s="19"/>
@@ -4413,7 +4375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" s="19"/>
       <c r="B153" s="19"/>
       <c r="C153" s="19"/>
@@ -4435,7 +4397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" s="19"/>
       <c r="B154" s="19"/>
       <c r="C154" s="19"/>
@@ -4457,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" s="19"/>
       <c r="B155" s="19"/>
       <c r="C155" s="19"/>
@@ -4479,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" s="19"/>
       <c r="B156" s="19"/>
       <c r="C156" s="19"/>
@@ -4501,7 +4463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" s="19"/>
       <c r="B157" s="19"/>
       <c r="C157" s="19"/>
@@ -4523,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" s="19"/>
       <c r="B158" s="19"/>
       <c r="C158" s="19"/>
@@ -4545,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" s="19"/>
       <c r="B159" s="19"/>
       <c r="C159" s="19"/>
@@ -4567,7 +4529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" s="19"/>
       <c r="B160" s="19"/>
       <c r="C160" s="19"/>
@@ -4589,7 +4551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" s="19"/>
       <c r="B161" s="19"/>
       <c r="C161" s="19"/>
@@ -4611,7 +4573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" s="19"/>
       <c r="B162" s="19"/>
       <c r="C162" s="19"/>
@@ -4633,7 +4595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" s="19"/>
       <c r="B163" s="19"/>
       <c r="C163" s="19"/>
@@ -4655,7 +4617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" s="19"/>
       <c r="B164" s="19"/>
       <c r="C164" s="19"/>
@@ -4677,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="19"/>
       <c r="B165" s="19"/>
       <c r="C165" s="19"/>
@@ -4699,7 +4661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" s="19"/>
       <c r="B166" s="19"/>
       <c r="C166" s="19"/>
@@ -4721,7 +4683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" s="19"/>
       <c r="B167" s="19"/>
       <c r="C167" s="19"/>
@@ -4743,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" s="19"/>
       <c r="B168" s="19"/>
       <c r="C168" s="19"/>
@@ -4765,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" s="19"/>
       <c r="B169" s="19"/>
       <c r="C169" s="19"/>
@@ -4787,7 +4749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" s="19"/>
       <c r="B170" s="19"/>
       <c r="C170" s="19"/>
@@ -4809,7 +4771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" s="19"/>
       <c r="B171" s="19"/>
       <c r="C171" s="19"/>
@@ -4831,7 +4793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" s="19"/>
       <c r="B172" s="19"/>
       <c r="C172" s="19"/>
@@ -4853,7 +4815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" s="19"/>
       <c r="B173" s="19"/>
       <c r="C173" s="19"/>
@@ -4875,7 +4837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" s="19"/>
       <c r="B174" s="19"/>
       <c r="C174" s="19"/>
@@ -4897,7 +4859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" s="19"/>
       <c r="B175" s="19"/>
       <c r="C175" s="19"/>
@@ -4919,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" s="19"/>
       <c r="B176" s="19"/>
       <c r="C176" s="19"/>
@@ -4941,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="19"/>
       <c r="B177" s="19"/>
       <c r="C177" s="19"/>
@@ -4963,7 +4925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="19"/>
       <c r="B178" s="19"/>
       <c r="C178" s="19"/>
@@ -4985,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="19"/>
       <c r="B179" s="19"/>
       <c r="C179" s="19"/>
@@ -5007,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="19"/>
       <c r="B180" s="19"/>
       <c r="C180" s="19"/>
@@ -5029,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="19"/>
       <c r="B181" s="19"/>
       <c r="C181" s="19"/>
@@ -5051,7 +5013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="19"/>
       <c r="B182" s="19"/>
       <c r="C182" s="19"/>
@@ -5073,7 +5035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="19"/>
       <c r="B183" s="19"/>
       <c r="C183" s="19"/>
@@ -5095,7 +5057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="19"/>
       <c r="B184" s="19"/>
       <c r="C184" s="19"/>
@@ -5117,7 +5079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="19"/>
       <c r="B185" s="19"/>
       <c r="C185" s="19"/>
@@ -5139,7 +5101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="19"/>
       <c r="B186" s="19"/>
       <c r="C186" s="19"/>
@@ -5161,7 +5123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="19"/>
       <c r="B187" s="19"/>
       <c r="C187" s="19"/>
@@ -5183,7 +5145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="19"/>
       <c r="B188" s="19"/>
       <c r="C188" s="19"/>
@@ -5205,7 +5167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="19"/>
       <c r="B189" s="19"/>
       <c r="C189" s="19"/>
@@ -5227,7 +5189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="19"/>
       <c r="B190" s="19"/>
       <c r="C190" s="19"/>
@@ -5249,7 +5211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="19"/>
       <c r="B191" s="19"/>
       <c r="C191" s="19"/>
@@ -5271,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="19"/>
       <c r="B192" s="19"/>
       <c r="C192" s="19"/>
@@ -5293,7 +5255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A193" s="19"/>
       <c r="B193" s="19"/>
       <c r="C193" s="19"/>
@@ -5315,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A194" s="19"/>
       <c r="B194" s="19"/>
       <c r="C194" s="19"/>
@@ -5337,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A195" s="19"/>
       <c r="B195" s="19"/>
       <c r="C195" s="19"/>
@@ -5359,7 +5321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A196" s="19"/>
       <c r="B196" s="19"/>
       <c r="C196" s="19"/>
@@ -5381,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A197" s="19"/>
       <c r="B197" s="19"/>
       <c r="C197" s="19"/>
@@ -5403,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A198" s="19"/>
       <c r="B198" s="19"/>
       <c r="C198" s="19"/>
@@ -5425,7 +5387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199" s="19"/>
       <c r="B199" s="19"/>
       <c r="C199" s="19"/>
@@ -5447,7 +5409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200" s="19"/>
       <c r="B200" s="19"/>
       <c r="C200" s="19"/>
@@ -5469,7 +5431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A201" s="19"/>
       <c r="B201" s="19"/>
       <c r="C201" s="19"/>
@@ -5491,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A202" s="19"/>
       <c r="B202" s="19"/>
       <c r="C202" s="19"/>
@@ -5513,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A203" s="19"/>
       <c r="B203" s="19"/>
       <c r="C203" s="19"/>
@@ -5535,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A204" s="19"/>
       <c r="B204" s="19"/>
       <c r="C204" s="19"/>
@@ -5557,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A205" s="19"/>
       <c r="B205" s="19"/>
       <c r="C205" s="19"/>
@@ -5579,7 +5541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A206" s="19"/>
       <c r="B206" s="19"/>
       <c r="C206" s="19"/>
@@ -5601,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A207" s="19"/>
       <c r="B207" s="19"/>
       <c r="C207" s="19"/>
@@ -5623,7 +5585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A208" s="19"/>
       <c r="B208" s="19"/>
       <c r="C208" s="19"/>
@@ -5645,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A209" s="19"/>
       <c r="B209" s="19"/>
       <c r="C209" s="19"/>
@@ -5667,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A210" s="19"/>
       <c r="B210" s="19"/>
       <c r="C210" s="19"/>
@@ -5689,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A211" s="19"/>
       <c r="B211" s="19"/>
       <c r="C211" s="19"/>
@@ -5711,7 +5673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A212" s="19"/>
       <c r="B212" s="19"/>
       <c r="C212" s="19"/>
@@ -5733,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A213" s="19"/>
       <c r="B213" s="19"/>
       <c r="C213" s="19"/>
@@ -5755,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A214" s="19"/>
       <c r="B214" s="19"/>
       <c r="C214" s="19"/>
@@ -5777,7 +5739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A215" s="19"/>
       <c r="B215" s="19"/>
       <c r="C215" s="19"/>
@@ -5799,7 +5761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A216" s="19"/>
       <c r="B216" s="19"/>
       <c r="C216" s="19"/>
@@ -5821,7 +5783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A217" s="19"/>
       <c r="B217" s="19"/>
       <c r="C217" s="19"/>
@@ -5843,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A218" s="19"/>
       <c r="B218" s="19"/>
       <c r="C218" s="19"/>
@@ -5865,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A219" s="19"/>
       <c r="B219" s="19"/>
       <c r="C219" s="19"/>
@@ -5887,7 +5849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A220" s="19"/>
       <c r="B220" s="19"/>
       <c r="C220" s="19"/>
@@ -5909,7 +5871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A221" s="19"/>
       <c r="B221" s="19"/>
       <c r="C221" s="19"/>
@@ -5931,7 +5893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A222" s="19"/>
       <c r="B222" s="19"/>
       <c r="C222" s="19"/>
@@ -5953,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A223" s="19"/>
       <c r="B223" s="19"/>
       <c r="C223" s="19"/>
@@ -5975,7 +5937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A224" s="19"/>
       <c r="B224" s="19"/>
       <c r="C224" s="19"/>
@@ -5997,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A225" s="19"/>
       <c r="B225" s="19"/>
       <c r="C225" s="19"/>
@@ -6019,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A226" s="19"/>
       <c r="B226" s="19"/>
       <c r="C226" s="19"/>
@@ -6041,7 +6003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A227" s="19"/>
       <c r="B227" s="19"/>
       <c r="C227" s="19"/>
@@ -6063,7 +6025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A228" s="19"/>
       <c r="B228" s="19"/>
       <c r="C228" s="19"/>
@@ -6085,7 +6047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A229" s="19"/>
       <c r="B229" s="19"/>
       <c r="C229" s="19"/>
@@ -6107,7 +6069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A230" s="19"/>
       <c r="B230" s="19"/>
       <c r="C230" s="19"/>
@@ -6129,7 +6091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A231" s="19"/>
       <c r="B231" s="19"/>
       <c r="C231" s="19"/>
@@ -6151,7 +6113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A232" s="19"/>
       <c r="B232" s="19"/>
       <c r="C232" s="19"/>
@@ -6173,7 +6135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A233" s="19"/>
       <c r="B233" s="19"/>
       <c r="C233" s="19"/>
@@ -6195,7 +6157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A234" s="19"/>
       <c r="B234" s="19"/>
       <c r="C234" s="19"/>
@@ -6217,7 +6179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A235" s="19"/>
       <c r="B235" s="19"/>
       <c r="C235" s="19"/>
@@ -6239,7 +6201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A236" s="19"/>
       <c r="B236" s="19"/>
       <c r="C236" s="19"/>
@@ -6261,7 +6223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A237" s="19"/>
       <c r="B237" s="19"/>
       <c r="C237" s="19"/>
@@ -6283,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A238" s="19"/>
       <c r="B238" s="19"/>
       <c r="C238" s="19"/>
@@ -6305,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A239" s="19"/>
       <c r="B239" s="19"/>
       <c r="C239" s="19"/>
@@ -6327,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A240" s="19"/>
       <c r="B240" s="19"/>
       <c r="C240" s="19"/>
@@ -6349,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A241" s="19"/>
       <c r="B241" s="19"/>
       <c r="C241" s="19"/>
@@ -6371,7 +6333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A242" s="19"/>
       <c r="B242" s="19"/>
       <c r="C242" s="19"/>
@@ -6393,7 +6355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A243" s="19"/>
       <c r="B243" s="19"/>
       <c r="C243" s="19"/>
@@ -6415,7 +6377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A244" s="19"/>
       <c r="B244" s="19"/>
       <c r="C244" s="19"/>
@@ -6437,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A245" s="19"/>
       <c r="B245" s="19"/>
       <c r="C245" s="19"/>
@@ -6459,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A246" s="19"/>
       <c r="B246" s="19"/>
       <c r="C246" s="19"/>
@@ -6481,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A247" s="19"/>
       <c r="B247" s="19"/>
       <c r="C247" s="19"/>
@@ -6503,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A248" s="19"/>
       <c r="B248" s="19"/>
       <c r="C248" s="19"/>
@@ -6525,7 +6487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A249" s="19"/>
       <c r="B249" s="19"/>
       <c r="C249" s="19"/>
@@ -6547,7 +6509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A250" s="19"/>
       <c r="B250" s="19"/>
       <c r="C250" s="19"/>
@@ -6569,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A251" s="19"/>
       <c r="B251" s="19"/>
       <c r="C251" s="19"/>
@@ -6591,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A252" s="19"/>
       <c r="B252" s="19"/>
       <c r="C252" s="19"/>
@@ -6613,7 +6575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A253" s="19"/>
       <c r="B253" s="19"/>
       <c r="C253" s="19"/>
@@ -6635,7 +6597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A254" s="19"/>
       <c r="B254" s="19"/>
       <c r="C254" s="19"/>
@@ -6657,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A255" s="19"/>
       <c r="B255" s="19"/>
       <c r="C255" s="19"/>
@@ -6679,7 +6641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A256" s="19"/>
       <c r="B256" s="19"/>
       <c r="C256" s="19"/>
@@ -6701,7 +6663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A257" s="19"/>
       <c r="B257" s="19"/>
       <c r="C257" s="19"/>
@@ -6723,7 +6685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A258" s="19"/>
       <c r="B258" s="19"/>
       <c r="C258" s="19"/>
@@ -6745,7 +6707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A259" s="19"/>
       <c r="B259" s="19"/>
       <c r="C259" s="19"/>
@@ -6767,7 +6729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A260" s="19"/>
       <c r="B260" s="19"/>
       <c r="C260" s="19"/>
@@ -6789,7 +6751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A261" s="19"/>
       <c r="B261" s="19"/>
       <c r="C261" s="19"/>
@@ -6811,7 +6773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A262" s="19"/>
       <c r="B262" s="19"/>
       <c r="C262" s="19"/>
@@ -6833,7 +6795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A263" s="19"/>
       <c r="B263" s="19"/>
       <c r="C263" s="19"/>
@@ -6855,7 +6817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A264" s="19"/>
       <c r="B264" s="19"/>
       <c r="C264" s="19"/>
@@ -6877,7 +6839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A265" s="19"/>
       <c r="B265" s="19"/>
       <c r="C265" s="19"/>
@@ -6899,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A266" s="19"/>
       <c r="B266" s="19"/>
       <c r="C266" s="19"/>
@@ -6921,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A267" s="19"/>
       <c r="B267" s="19"/>
       <c r="C267" s="19"/>
@@ -6943,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A268" s="19"/>
       <c r="B268" s="19"/>
       <c r="C268" s="19"/>
@@ -6965,7 +6927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A269" s="19"/>
       <c r="B269" s="19"/>
       <c r="C269" s="19"/>
@@ -6987,7 +6949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A270" s="19"/>
       <c r="B270" s="19"/>
       <c r="C270" s="19"/>
@@ -7009,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A271" s="19"/>
       <c r="B271" s="19"/>
       <c r="C271" s="19"/>
@@ -7031,7 +6993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" s="19"/>
       <c r="B272" s="19"/>
       <c r="C272" s="19"/>
@@ -7053,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" s="19"/>
       <c r="B273" s="19"/>
       <c r="C273" s="19"/>
@@ -7075,7 +7037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" s="19"/>
       <c r="B274" s="19"/>
       <c r="C274" s="19"/>
@@ -7097,7 +7059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" s="19"/>
       <c r="B275" s="19"/>
       <c r="C275" s="19"/>
@@ -7119,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" s="19"/>
       <c r="B276" s="19"/>
       <c r="C276" s="19"/>
@@ -7141,7 +7103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" s="19"/>
       <c r="B277" s="19"/>
       <c r="C277" s="19"/>
@@ -7163,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" s="19"/>
       <c r="B278" s="19"/>
       <c r="C278" s="19"/>
@@ -7185,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" s="19"/>
       <c r="B279" s="19"/>
       <c r="C279" s="19"/>
@@ -7207,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" s="19"/>
       <c r="B280" s="19"/>
       <c r="C280" s="19"/>
@@ -7229,7 +7191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" s="19"/>
       <c r="B281" s="19"/>
       <c r="C281" s="19"/>
@@ -7251,7 +7213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" s="19"/>
       <c r="B282" s="19"/>
       <c r="C282" s="19"/>
@@ -7273,7 +7235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" s="19"/>
       <c r="B283" s="19"/>
       <c r="C283" s="19"/>
@@ -7295,7 +7257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" s="19"/>
       <c r="B284" s="19"/>
       <c r="C284" s="19"/>
@@ -7317,7 +7279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" s="19"/>
       <c r="B285" s="19"/>
       <c r="C285" s="19"/>
@@ -7339,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" s="19"/>
       <c r="B286" s="19"/>
       <c r="C286" s="19"/>
@@ -7361,7 +7323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" s="19"/>
       <c r="B287" s="19"/>
       <c r="C287" s="19"/>
@@ -7383,7 +7345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" s="19"/>
       <c r="B288" s="19"/>
       <c r="C288" s="19"/>
@@ -7405,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A289" s="19"/>
       <c r="B289" s="19"/>
       <c r="C289" s="19"/>
@@ -7427,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A290" s="19"/>
       <c r="B290" s="19"/>
       <c r="C290" s="19"/>
@@ -7449,7 +7411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A291" s="19"/>
       <c r="B291" s="19"/>
       <c r="C291" s="19"/>
@@ -7471,7 +7433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A292" s="19"/>
       <c r="B292" s="19"/>
       <c r="C292" s="19"/>
@@ -7493,7 +7455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A293" s="19"/>
       <c r="B293" s="19"/>
       <c r="C293" s="19"/>
@@ -7515,7 +7477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A294" s="19"/>
       <c r="B294" s="19"/>
       <c r="C294" s="19"/>
@@ -7537,7 +7499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A295" s="19"/>
       <c r="B295" s="19"/>
       <c r="C295" s="19"/>
@@ -7559,7 +7521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A296" s="19"/>
       <c r="B296" s="19"/>
       <c r="C296" s="19"/>
@@ -7581,7 +7543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A297" s="19"/>
       <c r="B297" s="19"/>
       <c r="C297" s="19"/>
@@ -7603,7 +7565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A298" s="19"/>
       <c r="B298" s="19"/>
       <c r="C298" s="19"/>
@@ -7625,7 +7587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A299" s="19"/>
       <c r="B299" s="19"/>
       <c r="C299" s="19"/>
@@ -7647,7 +7609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A300" s="19"/>
       <c r="B300" s="19"/>
       <c r="C300" s="19"/>
@@ -7669,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A301" s="19"/>
       <c r="B301" s="19"/>
       <c r="C301" s="19"/>
@@ -7691,7 +7653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A302" s="19"/>
       <c r="B302" s="19"/>
       <c r="C302" s="19"/>
@@ -7713,7 +7675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A303" s="19"/>
       <c r="B303" s="19"/>
       <c r="C303" s="19"/>
@@ -7735,7 +7697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" s="19"/>
       <c r="B304" s="19"/>
       <c r="C304" s="19"/>
@@ -7757,7 +7719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" s="19"/>
       <c r="B305" s="19"/>
       <c r="C305" s="19"/>
@@ -7779,7 +7741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" s="19"/>
       <c r="B306" s="19"/>
       <c r="C306" s="19"/>
@@ -7801,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" s="19"/>
       <c r="B307" s="19"/>
       <c r="C307" s="19"/>
@@ -7823,7 +7785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A308" s="19"/>
       <c r="B308" s="19"/>
       <c r="C308" s="19"/>
@@ -7845,7 +7807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A309" s="19"/>
       <c r="B309" s="19"/>
       <c r="C309" s="19"/>
@@ -7867,7 +7829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A310" s="19"/>
       <c r="B310" s="19"/>
       <c r="C310" s="19"/>
@@ -7889,7 +7851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" s="19"/>
       <c r="B311" s="19"/>
       <c r="C311" s="19"/>
@@ -7911,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A312" s="19"/>
       <c r="B312" s="19"/>
       <c r="C312" s="19"/>
@@ -7933,7 +7895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A313" s="19"/>
       <c r="B313" s="19"/>
       <c r="C313" s="19"/>
@@ -7955,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A314" s="19"/>
       <c r="B314" s="19"/>
       <c r="C314" s="19"/>
@@ -7977,7 +7939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A315" s="19"/>
       <c r="B315" s="19"/>
       <c r="C315" s="19"/>
@@ -7999,7 +7961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A316" s="19"/>
       <c r="B316" s="19"/>
       <c r="C316" s="19"/>
@@ -8021,7 +7983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" s="19"/>
       <c r="B317" s="19"/>
       <c r="C317" s="19"/>
@@ -8043,7 +8005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A318" s="19"/>
       <c r="B318" s="19"/>
       <c r="C318" s="19"/>
@@ -8065,7 +8027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A319" s="19"/>
       <c r="B319" s="19"/>
       <c r="C319" s="19"/>
@@ -8087,7 +8049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A320" s="19"/>
       <c r="B320" s="19"/>
       <c r="C320" s="19"/>
@@ -8109,7 +8071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A321" s="19"/>
       <c r="B321" s="19"/>
       <c r="C321" s="19"/>
@@ -8131,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" s="19"/>
       <c r="B322" s="19"/>
       <c r="C322" s="19"/>
@@ -8153,7 +8115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A323" s="19"/>
       <c r="B323" s="19"/>
       <c r="C323" s="19"/>
@@ -8175,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A324" s="19"/>
       <c r="B324" s="19"/>
       <c r="C324" s="19"/>
@@ -8197,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A325" s="19"/>
       <c r="B325" s="19"/>
       <c r="C325" s="19"/>
@@ -8219,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A326" s="19"/>
       <c r="B326" s="19"/>
       <c r="C326" s="19"/>
@@ -8241,7 +8203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A327" s="19"/>
       <c r="B327" s="19"/>
       <c r="C327" s="19"/>
@@ -8263,7 +8225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A328" s="19"/>
       <c r="B328" s="19"/>
       <c r="C328" s="19"/>
@@ -8285,7 +8247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A329" s="19"/>
       <c r="B329" s="19"/>
       <c r="C329" s="19"/>
@@ -8307,7 +8269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A330" s="19"/>
       <c r="B330" s="19"/>
       <c r="C330" s="19"/>
@@ -8329,7 +8291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A331" s="19"/>
       <c r="B331" s="19"/>
       <c r="C331" s="19"/>
@@ -8351,7 +8313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A332" s="19"/>
       <c r="B332" s="19"/>
       <c r="C332" s="19"/>
@@ -8373,7 +8335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A333" s="19"/>
       <c r="B333" s="19"/>
       <c r="C333" s="19"/>
@@ -8395,7 +8357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A334" s="19"/>
       <c r="B334" s="19"/>
       <c r="C334" s="19"/>
@@ -8417,7 +8379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A335" s="19"/>
       <c r="B335" s="19"/>
       <c r="C335" s="19"/>
@@ -8439,7 +8401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A336" s="19"/>
       <c r="B336" s="19"/>
       <c r="C336" s="19"/>
@@ -8461,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A337" s="19"/>
       <c r="B337" s="19"/>
       <c r="C337" s="19"/>
@@ -8483,7 +8445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A338" s="19"/>
       <c r="B338" s="19"/>
       <c r="C338" s="19"/>
@@ -8505,7 +8467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A339" s="19"/>
       <c r="B339" s="19"/>
       <c r="C339" s="19"/>
@@ -8527,7 +8489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A340" s="19"/>
       <c r="B340" s="19"/>
       <c r="C340" s="19"/>
@@ -8549,7 +8511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A341" s="19"/>
       <c r="B341" s="19"/>
       <c r="C341" s="19"/>
@@ -8571,7 +8533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A342" s="19"/>
       <c r="B342" s="19"/>
       <c r="C342" s="19"/>
@@ -8593,7 +8555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A343" s="19"/>
       <c r="B343" s="19"/>
       <c r="C343" s="19"/>
@@ -8615,7 +8577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A344" s="19"/>
       <c r="B344" s="19"/>
       <c r="C344" s="19"/>
@@ -8637,7 +8599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A345" s="19"/>
       <c r="B345" s="19"/>
       <c r="C345" s="19"/>
@@ -8659,7 +8621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A346" s="19"/>
       <c r="B346" s="19"/>
       <c r="C346" s="19"/>
@@ -8681,7 +8643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A347" s="19"/>
       <c r="B347" s="19"/>
       <c r="C347" s="19"/>
@@ -8703,7 +8665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A348" s="19"/>
       <c r="B348" s="19"/>
       <c r="C348" s="19"/>
@@ -8725,7 +8687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A349" s="19"/>
       <c r="B349" s="19"/>
       <c r="C349" s="19"/>
@@ -8747,7 +8709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A350" s="19"/>
       <c r="B350" s="19"/>
       <c r="C350" s="19"/>
@@ -8769,7 +8731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A351" s="19"/>
       <c r="B351" s="19"/>
       <c r="C351" s="19"/>
@@ -8791,7 +8753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A352" s="19"/>
       <c r="B352" s="19"/>
       <c r="C352" s="19"/>
@@ -8813,7 +8775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353" s="19"/>
       <c r="B353" s="19"/>
       <c r="C353" s="19"/>
@@ -8835,7 +8797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354" s="19"/>
       <c r="B354" s="19"/>
       <c r="C354" s="19"/>
@@ -8857,7 +8819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355" s="19"/>
       <c r="B355" s="19"/>
       <c r="C355" s="19"/>
@@ -8879,7 +8841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356" s="19"/>
       <c r="B356" s="19"/>
       <c r="C356" s="19"/>
@@ -8901,7 +8863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="19"/>
       <c r="B357" s="19"/>
       <c r="C357" s="19"/>
@@ -8923,7 +8885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" s="19"/>
       <c r="B358" s="19"/>
       <c r="C358" s="19"/>
@@ -8945,7 +8907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359" s="19"/>
       <c r="B359" s="19"/>
       <c r="C359" s="19"/>
@@ -8967,7 +8929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="360" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="19"/>
       <c r="B360" s="19"/>
       <c r="C360" s="19"/>
@@ -8990,7 +8952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A361" s="19"/>
       <c r="B361" s="19"/>
       <c r="C361" s="19"/>
@@ -9013,7 +8975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" s="19"/>
       <c r="B362" s="39"/>
       <c r="C362" s="19"/>
@@ -9022,7 +8984,7 @@
       <c r="H362" s="25"/>
       <c r="I362" s="40"/>
     </row>
-    <row r="363" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A363" s="19"/>
       <c r="B363" s="19"/>
       <c r="C363" s="19"/>
@@ -9039,7 +9001,7 @@
       </c>
       <c r="J363"/>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364" s="19"/>
       <c r="B364" s="19"/>
       <c r="C364" s="19"/>
@@ -9048,7 +9010,7 @@
       <c r="H364" s="25"/>
       <c r="I364" s="25"/>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365" s="19"/>
       <c r="B365" s="19"/>
       <c r="C365" s="48" t="s">
@@ -9059,7 +9021,7 @@
       <c r="H365" s="25"/>
       <c r="I365" s="25"/>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366" s="19"/>
       <c r="B366" s="19"/>
       <c r="C366" s="19"/>
@@ -9068,7 +9030,7 @@
       <c r="H366" s="25"/>
       <c r="I366" s="25"/>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367" s="19"/>
       <c r="B367" s="19"/>
       <c r="C367" s="19"/>
@@ -9090,7 +9052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368" s="19"/>
       <c r="B368" s="19"/>
       <c r="C368" s="19"/>
@@ -9114,7 +9076,7 @@
       </c>
       <c r="J368"/>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A369" s="19"/>
       <c r="B369" s="19"/>
       <c r="C369" s="19"/>
@@ -9136,7 +9098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A370" s="19"/>
       <c r="B370" s="19"/>
       <c r="C370" s="19"/>
@@ -9158,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A371" s="19"/>
       <c r="B371" s="19"/>
       <c r="C371" s="19"/>
@@ -9180,7 +9142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A372" s="19"/>
       <c r="B372" s="19"/>
       <c r="C372" s="19"/>
@@ -9189,7 +9151,7 @@
       <c r="H372" s="25"/>
       <c r="I372" s="41"/>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A373" s="19"/>
       <c r="B373" s="19"/>
       <c r="C373" s="19"/>
@@ -9203,7 +9165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A374" s="19"/>
       <c r="B374" s="19"/>
       <c r="C374" s="19"/>
@@ -9212,7 +9174,7 @@
       <c r="H374" s="25"/>
       <c r="I374" s="25"/>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A375" s="19"/>
       <c r="B375" s="19"/>
       <c r="C375" s="48" t="s">
@@ -9223,14 +9185,14 @@
       <c r="H375" s="25"/>
       <c r="I375" s="25"/>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B376" s="19"/>
       <c r="D376" s="9"/>
       <c r="G376" s="25"/>
       <c r="H376" s="9"/>
       <c r="I376" s="10"/>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A377" s="8"/>
       <c r="B377" s="8"/>
       <c r="C377" s="8"/>
@@ -9253,7 +9215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B378" s="19"/>
       <c r="D378" s="9">
         <v>0</v>
@@ -9273,7 +9235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B379" s="19"/>
       <c r="D379" s="9">
         <v>0</v>
@@ -9293,7 +9255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D380" s="9">
         <v>0</v>
       </c>
@@ -9312,7 +9274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B381" s="19"/>
       <c r="D381" s="9">
         <v>0</v>
@@ -9332,14 +9294,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B382" s="19"/>
       <c r="D382" s="9"/>
       <c r="G382" s="25"/>
       <c r="H382" s="9"/>
       <c r="I382" s="26"/>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D383" s="1"/>
       <c r="H383" s="13" t="s">
         <v>19</v>
@@ -9349,17 +9311,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D385" s="34"/>
       <c r="H385" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I385" s="6">
         <f>I383+I373+I363</f>
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A386" s="12"/>
       <c r="B386" s="12"/>
       <c r="C386" s="12"/>
@@ -9370,7 +9332,7 @@
       <c r="H386" s="18"/>
       <c r="I386" s="44"/>
     </row>
-    <row r="388" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C388" s="45" t="s">
         <v>49</v>
       </c>
@@ -9378,7 +9340,7 @@
       <c r="H388" s="20"/>
       <c r="I388" s="6"/>
     </row>
-    <row r="390" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:9" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A390" s="55" t="s">
         <v>2</v>
       </c>
@@ -9407,7 +9369,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A391" s="72"/>
       <c r="B391" s="72"/>
       <c r="C391" s="72"/>
@@ -9430,7 +9392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B392" s="19"/>
       <c r="D392" s="46">
         <v>0</v>
@@ -9450,7 +9412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A393" s="59"/>
       <c r="B393" s="39"/>
       <c r="C393" s="59"/>
@@ -9473,7 +9435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A394" s="59"/>
       <c r="B394" s="39"/>
       <c r="C394" s="59"/>
@@ -9496,7 +9458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A395" s="59"/>
       <c r="B395" s="39"/>
       <c r="C395" s="59"/>
@@ -9519,7 +9481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A396" s="59"/>
       <c r="B396" s="39"/>
       <c r="C396" s="59"/>
@@ -9542,7 +9504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A397" s="59"/>
       <c r="B397" s="39"/>
       <c r="C397" s="59"/>
@@ -9565,7 +9527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:9" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:9" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B398" s="39"/>
       <c r="D398" s="60">
         <v>0</v>
@@ -9585,7 +9547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:9" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:9" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B399" s="39"/>
       <c r="D399" s="60">
         <v>0</v>
@@ -9605,7 +9567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:9" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:9" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B400" s="39"/>
       <c r="D400" s="60">
         <v>0</v>
@@ -9625,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:10" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:10" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B401" s="39"/>
       <c r="D401" s="60">
         <v>0</v>
@@ -9645,7 +9607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:10" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:10" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B402" s="39"/>
       <c r="D402" s="60">
         <v>0</v>
@@ -9665,7 +9627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="403" spans="1:10" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:10" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A403" s="39"/>
       <c r="B403" s="39"/>
       <c r="C403" s="39"/>
@@ -9687,14 +9649,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="404" spans="1:10" s="59" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:10" s="59" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="B404" s="39"/>
       <c r="D404" s="62"/>
       <c r="G404" s="61"/>
       <c r="H404" s="62"/>
       <c r="I404" s="61"/>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D405" s="9"/>
       <c r="G405" s="25"/>
       <c r="H405" s="20" t="s">
@@ -9706,7 +9668,7 @@
       </c>
       <c r="J405" s="47"/>
     </row>
-    <row r="406" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A406" s="12"/>
       <c r="B406" s="12"/>
       <c r="C406" s="12"/>
@@ -9717,12 +9679,12 @@
       <c r="H406" s="18"/>
       <c r="I406" s="44"/>
     </row>
-    <row r="408" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C408" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="410" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10" s="58" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A410" s="55" t="s">
         <v>2</v>
       </c>
@@ -9751,7 +9713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A411" s="8"/>
       <c r="B411" s="73"/>
       <c r="C411" s="74"/>
@@ -9774,7 +9736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A412" s="12"/>
       <c r="B412" s="12"/>
       <c r="C412" s="12"/>
@@ -9785,12 +9747,12 @@
       <c r="H412" s="18"/>
       <c r="I412" s="44"/>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D414" s="1"/>
       <c r="H414" s="1"/>
       <c r="I414" s="25"/>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D415" s="1"/>
       <c r="H415" s="20" t="s">
         <v>24</v>
@@ -9800,7 +9762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="417" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C417" s="13" t="s">
         <v>25</v>
       </c>
@@ -9812,7 +9774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="418" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="418" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D418" s="34" t="s">
         <v>27</v>
       </c>
@@ -9821,16 +9783,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="419" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D419" s="34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I419" s="25">
         <f>I100</f>
         <v>0</v>
       </c>
     </row>
-    <row r="420" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="420" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D420" s="34" t="s">
         <v>28</v>
       </c>
@@ -9839,7 +9801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="421" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D421" s="34" t="s">
         <v>23</v>
       </c>
@@ -9849,9 +9811,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="422" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="422" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D422" s="34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G422" s="25"/>
       <c r="H422" s="9"/>
@@ -9860,7 +9822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="423" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D423" s="3"/>
       <c r="H423" s="13" t="s">
         <v>29</v>
@@ -9870,13 +9832,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="426" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C426" s="13" t="s">
         <v>30</v>
       </c>
       <c r="E426" s="2"/>
     </row>
-    <row r="427" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="427" spans="3:9" x14ac:dyDescent="0.2">
       <c r="F427" s="2" t="s">
         <v>31</v>
       </c>
@@ -9884,7 +9846,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="428" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="428" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D428" s="34" t="s">
         <v>26</v>
       </c>
@@ -9893,11 +9855,11 @@
         <v>56.69</v>
       </c>
       <c r="I428" s="25">
-        <f>G428*F428</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="429" spans="3:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I428:I433" si="28">G428*F428</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="429" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D429" s="34" t="s">
         <v>27</v>
       </c>
@@ -9906,17 +9868,24 @@
         <v>30.22</v>
       </c>
       <c r="I429" s="25">
-        <f>G429*F429</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="430" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D430" s="34"/>
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="430" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D430" s="34" t="s">
+        <v>53</v>
+      </c>
       <c r="F430" s="14"/>
-      <c r="G430" s="75"/>
-      <c r="I430" s="25"/>
-    </row>
-    <row r="431" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G430" s="75">
+        <v>0</v>
+      </c>
+      <c r="I430" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="431" spans="3:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D431" s="34" t="s">
         <v>28</v>
       </c>
@@ -9925,11 +9894,11 @@
         <v>35.619999999999997</v>
       </c>
       <c r="I431" s="25">
-        <f>G431*F431</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="432" spans="3:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="432" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D432" s="34" t="s">
         <v>33</v>
       </c>
@@ -9938,11 +9907,11 @@
         <v>40.840000000000003</v>
       </c>
       <c r="I432" s="25">
-        <f>G432*F432</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="433" spans="3:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="433" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D433" s="34" t="s">
         <v>34</v>
       </c>
@@ -9951,11 +9920,11 @@
         <v>36</v>
       </c>
       <c r="I433" s="25">
-        <f>G433*F433</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="434" spans="3:9" x14ac:dyDescent="0.25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="434" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D434" s="3" t="s">
         <v>35</v>
       </c>
@@ -9972,12 +9941,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="435" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="435" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D435" s="3"/>
       <c r="F435" s="14"/>
       <c r="G435" s="21"/>
     </row>
-    <row r="436" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="436" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C436" s="13" t="s">
         <v>37</v>
       </c>
@@ -9986,12 +9955,12 @@
       <c r="F436" s="14"/>
       <c r="G436" s="21"/>
     </row>
-    <row r="437" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="437" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D437" s="3"/>
       <c r="F437" s="14"/>
       <c r="G437" s="21"/>
     </row>
-    <row r="438" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="438" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D438" s="34" t="s">
         <v>38</v>
       </c>
@@ -10001,7 +9970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="439" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="439" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D439" s="34" t="s">
         <v>39</v>
       </c>
@@ -10011,7 +9980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="440" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="440" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D440" s="34" t="s">
         <v>40</v>
       </c>
@@ -10021,7 +9990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="441" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="441" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D441" s="34"/>
       <c r="F441" s="14"/>
       <c r="G441" s="14"/>
@@ -10029,12 +9998,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="442" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="442" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I442" s="42">
         <v>0</v>
       </c>
     </row>
-    <row r="443" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="443" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D443" s="3"/>
       <c r="H443" s="13" t="s">
         <v>41</v>
@@ -10044,7 +10013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="446" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="446" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D446" s="3"/>
       <c r="G446" s="13" t="s">
         <v>42</v>
@@ -10054,14 +10023,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="448" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D448" s="3"/>
       <c r="G448" s="13" t="s">
         <v>43</v>
       </c>
       <c r="I448" s="29"/>
     </row>
-    <row r="450" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="450" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D450" s="3"/>
       <c r="G450" s="13" t="s">
         <v>44</v>
@@ -10071,7 +10040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="452" spans="3:9" x14ac:dyDescent="0.2">
       <c r="G452" s="13" t="s">
         <v>45</v>
       </c>
@@ -10080,28 +10049,28 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="455" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="455" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C455" s="3"/>
       <c r="D455" s="1"/>
       <c r="H455" s="1"/>
       <c r="I455" s="25"/>
     </row>
-    <row r="456" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="456" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I456" s="25"/>
     </row>
-    <row r="457" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="457" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I457" s="25"/>
     </row>
-    <row r="458" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="458" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I458" s="25"/>
     </row>
-    <row r="459" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="459" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I459" s="25"/>
     </row>
-    <row r="460" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="460" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I460" s="25"/>
     </row>
-    <row r="461" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="461" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I461" s="25"/>
     </row>
   </sheetData>

</xml_diff>